<commit_message>
added 1990/91 to excel file
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/pp12-92-seasons/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5828952C-DDE4-4E48-A763-0BA32A5364C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDAEB17-B5FF-CB45-AF05-384296B86AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="1991-92" sheetId="7" r:id="rId1"/>
-    <sheet name="Sheet11" sheetId="15" r:id="rId2"/>
+    <sheet name="1990-91" sheetId="16" r:id="rId1"/>
+    <sheet name="1991-92" sheetId="7" r:id="rId2"/>
     <sheet name="1992-93" sheetId="11" r:id="rId3"/>
     <sheet name="1993-94" sheetId="14" r:id="rId4"/>
     <sheet name="1994-95" sheetId="1" r:id="rId5"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="78">
   <si>
     <t>11+</t>
   </si>
@@ -267,12 +267,21 @@
   <si>
     <t>14*</t>
   </si>
+  <si>
+    <t>Bishop</t>
+  </si>
+  <si>
+    <t>McCarrick</t>
+  </si>
+  <si>
+    <t>IMcNab</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,6 +294,19 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,9 +329,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,6 +647,2921 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B1DCE2-83C0-7043-83EC-E3BF8EDF97DC}">
+  <dimension ref="A1:T62"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:T62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3">
+        <v>14</v>
+      </c>
+      <c r="L2" s="3">
+        <v>3</v>
+      </c>
+      <c r="M2" s="3">
+        <v>4</v>
+      </c>
+      <c r="N2" s="3">
+        <v>7</v>
+      </c>
+      <c r="O2" s="3">
+        <v>10</v>
+      </c>
+      <c r="P2" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1</v>
+      </c>
+      <c r="R2" s="3">
+        <v>9</v>
+      </c>
+      <c r="S2" s="3">
+        <v>11</v>
+      </c>
+      <c r="T2" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>4</v>
+      </c>
+      <c r="N3" s="3">
+        <v>7</v>
+      </c>
+      <c r="O3" s="3">
+        <v>10</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3">
+        <v>9</v>
+      </c>
+      <c r="S3" s="3">
+        <v>11</v>
+      </c>
+      <c r="T3" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3">
+        <v>14</v>
+      </c>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3">
+        <v>12</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3">
+        <v>4</v>
+      </c>
+      <c r="N4" s="3">
+        <v>7</v>
+      </c>
+      <c r="O4" s="3">
+        <v>10</v>
+      </c>
+      <c r="P4" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>1</v>
+      </c>
+      <c r="R4" s="3">
+        <v>9</v>
+      </c>
+      <c r="S4" s="3">
+        <v>11</v>
+      </c>
+      <c r="T4" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3">
+        <v>12</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="M5" s="3">
+        <v>4</v>
+      </c>
+      <c r="N5" s="3">
+        <v>7</v>
+      </c>
+      <c r="O5" s="3">
+        <v>10</v>
+      </c>
+      <c r="P5" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3">
+        <v>9</v>
+      </c>
+      <c r="S5" s="3">
+        <v>11</v>
+      </c>
+      <c r="T5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3">
+        <v>12</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7</v>
+      </c>
+      <c r="O6" s="3">
+        <v>10</v>
+      </c>
+      <c r="P6" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>1</v>
+      </c>
+      <c r="R6" s="3">
+        <v>9</v>
+      </c>
+      <c r="S6" s="3">
+        <v>11</v>
+      </c>
+      <c r="T6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
+        <v>14</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3">
+        <v>4</v>
+      </c>
+      <c r="N7" s="3">
+        <v>7</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>1</v>
+      </c>
+      <c r="R7" s="3">
+        <v>9</v>
+      </c>
+      <c r="S7" s="3">
+        <v>11</v>
+      </c>
+      <c r="T7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3">
+        <v>12</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3">
+        <v>4</v>
+      </c>
+      <c r="N8" s="3">
+        <v>7</v>
+      </c>
+      <c r="O8" s="3">
+        <v>10</v>
+      </c>
+      <c r="P8" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>1</v>
+      </c>
+      <c r="R8" s="3">
+        <v>9</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3">
+        <v>14</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3">
+        <v>4</v>
+      </c>
+      <c r="N9" s="3">
+        <v>7</v>
+      </c>
+      <c r="O9" s="3">
+        <v>10</v>
+      </c>
+      <c r="P9" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>1</v>
+      </c>
+      <c r="R9" s="3">
+        <v>9</v>
+      </c>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3">
+        <v>8</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3">
+        <v>14</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3">
+        <v>3</v>
+      </c>
+      <c r="M10" s="3">
+        <v>4</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="3">
+        <v>10</v>
+      </c>
+      <c r="P10" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>1</v>
+      </c>
+      <c r="R10" s="3">
+        <v>9</v>
+      </c>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
+      <c r="G11" s="3">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>5</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3">
+        <v>14</v>
+      </c>
+      <c r="K11" s="3">
+        <v>12</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="3">
+        <v>10</v>
+      </c>
+      <c r="P11" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>1</v>
+      </c>
+      <c r="R11" s="3">
+        <v>9</v>
+      </c>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3">
+        <v>8</v>
+      </c>
+      <c r="G12" s="3">
+        <v>2</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="3">
+        <v>14</v>
+      </c>
+      <c r="J12" s="3">
+        <v>9</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3">
+        <v>3</v>
+      </c>
+      <c r="M12" s="3">
+        <v>4</v>
+      </c>
+      <c r="N12" s="3">
+        <v>7</v>
+      </c>
+      <c r="O12" s="3">
+        <v>10</v>
+      </c>
+      <c r="P12" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3">
+        <v>8</v>
+      </c>
+      <c r="G13" s="3">
+        <v>2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3">
+        <v>11</v>
+      </c>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3">
+        <v>3</v>
+      </c>
+      <c r="M13" s="3">
+        <v>4</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O13" s="3">
+        <v>10</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3">
+        <v>9</v>
+      </c>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>8</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3">
+        <v>11</v>
+      </c>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3">
+        <v>3</v>
+      </c>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O14" s="3">
+        <v>10</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
+        <v>9</v>
+      </c>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
+        <v>8</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>5</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3">
+        <v>7</v>
+      </c>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3">
+        <v>3</v>
+      </c>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3">
+        <v>10</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3">
+        <v>9</v>
+      </c>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>14</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3">
+        <v>7</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>3</v>
+      </c>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3">
+        <v>12</v>
+      </c>
+      <c r="O16" s="3">
+        <v>10</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
+        <v>9</v>
+      </c>
+      <c r="S16" s="3"/>
+      <c r="T16" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="3">
+        <v>2</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3">
+        <v>7</v>
+      </c>
+      <c r="K17" s="3">
+        <v>14</v>
+      </c>
+      <c r="L17" s="3">
+        <v>3</v>
+      </c>
+      <c r="M17" s="3">
+        <v>4</v>
+      </c>
+      <c r="N17" s="3">
+        <v>12</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>9</v>
+      </c>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>8</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3">
+        <v>5</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3">
+        <v>11</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3">
+        <v>3</v>
+      </c>
+      <c r="M18" s="3">
+        <v>4</v>
+      </c>
+      <c r="N18" s="3">
+        <v>7</v>
+      </c>
+      <c r="O18" s="3">
+        <v>10</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>9</v>
+      </c>
+      <c r="S18" s="3"/>
+      <c r="T18" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <v>11</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3">
+        <v>14</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3">
+        <v>3</v>
+      </c>
+      <c r="M19" s="3">
+        <v>4</v>
+      </c>
+      <c r="N19" s="3">
+        <v>7</v>
+      </c>
+      <c r="O19" s="3">
+        <v>10</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3">
+        <v>9</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3">
+        <v>11</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>8</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3">
+        <v>3</v>
+      </c>
+      <c r="M20" s="3">
+        <v>4</v>
+      </c>
+      <c r="N20" s="3">
+        <v>7</v>
+      </c>
+      <c r="O20" s="3">
+        <v>10</v>
+      </c>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>9</v>
+      </c>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
+      <c r="G21" s="3">
+        <v>2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3">
+        <v>4</v>
+      </c>
+      <c r="N21" s="3">
+        <v>7</v>
+      </c>
+      <c r="O21" s="3">
+        <v>10</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>9</v>
+      </c>
+      <c r="S21" s="3">
+        <v>11</v>
+      </c>
+      <c r="T21" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>14</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3">
+        <v>12</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3">
+        <v>4</v>
+      </c>
+      <c r="N22" s="3">
+        <v>7</v>
+      </c>
+      <c r="O22" s="3">
+        <v>10</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3">
+        <v>1</v>
+      </c>
+      <c r="R22" s="3">
+        <v>9</v>
+      </c>
+      <c r="S22" s="3">
+        <v>11</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+      <c r="I23" s="3">
+        <v>6</v>
+      </c>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3">
+        <v>14</v>
+      </c>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3">
+        <v>4</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O23" s="3">
+        <v>10</v>
+      </c>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3">
+        <v>9</v>
+      </c>
+      <c r="S23" s="3">
+        <v>11</v>
+      </c>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>8</v>
+      </c>
+      <c r="B24" s="3">
+        <v>3</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3">
+        <v>12</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3">
+        <v>14</v>
+      </c>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3">
+        <v>4</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O24" s="3">
+        <v>10</v>
+      </c>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3">
+        <v>9</v>
+      </c>
+      <c r="S24" s="3">
+        <v>11</v>
+      </c>
+      <c r="T24" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>8</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <v>9</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3">
+        <v>12</v>
+      </c>
+      <c r="G25" s="3">
+        <v>2</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="3">
+        <v>7</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3">
+        <v>4</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3">
+        <v>1</v>
+      </c>
+      <c r="R25" s="3">
+        <v>14</v>
+      </c>
+      <c r="S25" s="3">
+        <v>11</v>
+      </c>
+      <c r="T25" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>8</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>5</v>
+      </c>
+      <c r="I26" s="3">
+        <v>7</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3">
+        <v>4</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3">
+        <v>1</v>
+      </c>
+      <c r="R26" s="3">
+        <v>9</v>
+      </c>
+      <c r="S26" s="3">
+        <v>11</v>
+      </c>
+      <c r="T26" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3">
+        <v>3</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3">
+        <v>8</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I27" s="3">
+        <v>7</v>
+      </c>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3">
+        <v>4</v>
+      </c>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3">
+        <v>12</v>
+      </c>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3">
+        <v>1</v>
+      </c>
+      <c r="R27" s="3">
+        <v>9</v>
+      </c>
+      <c r="S27" s="3">
+        <v>11</v>
+      </c>
+      <c r="T27" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>8</v>
+      </c>
+      <c r="G28" s="3">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3">
+        <v>7</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3">
+        <v>4</v>
+      </c>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3">
+        <v>12</v>
+      </c>
+      <c r="P28" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3">
+        <v>9</v>
+      </c>
+      <c r="S28" s="3">
+        <v>11</v>
+      </c>
+      <c r="T28" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3">
+        <v>3</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3">
+        <v>8</v>
+      </c>
+      <c r="G29" s="3">
+        <v>2</v>
+      </c>
+      <c r="H29" s="3">
+        <v>5</v>
+      </c>
+      <c r="I29" s="3">
+        <v>7</v>
+      </c>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3">
+        <v>4</v>
+      </c>
+      <c r="N29" s="3">
+        <v>12</v>
+      </c>
+      <c r="O29" s="3">
+        <v>10</v>
+      </c>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3">
+        <v>1</v>
+      </c>
+      <c r="R29" s="3">
+        <v>9</v>
+      </c>
+      <c r="S29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T29" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>8</v>
+      </c>
+      <c r="G30" s="3">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>5</v>
+      </c>
+      <c r="I30" s="3">
+        <v>11</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3">
+        <v>4</v>
+      </c>
+      <c r="N30" s="3">
+        <v>7</v>
+      </c>
+      <c r="O30" s="3">
+        <v>10</v>
+      </c>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3">
+        <v>1</v>
+      </c>
+      <c r="R30" s="3">
+        <v>9</v>
+      </c>
+      <c r="S30" s="3"/>
+      <c r="T30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3">
+        <v>12</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3">
+        <v>8</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3">
+        <v>4</v>
+      </c>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O31" s="3">
+        <v>10</v>
+      </c>
+      <c r="P31" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>1</v>
+      </c>
+      <c r="R31" s="3">
+        <v>9</v>
+      </c>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>8</v>
+      </c>
+      <c r="G32" s="3">
+        <v>2</v>
+      </c>
+      <c r="H32" s="3">
+        <v>5</v>
+      </c>
+      <c r="I32" s="3">
+        <v>4</v>
+      </c>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3">
+        <v>7</v>
+      </c>
+      <c r="O32" s="3">
+        <v>10</v>
+      </c>
+      <c r="P32" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>1</v>
+      </c>
+      <c r="R32" s="3">
+        <v>9</v>
+      </c>
+      <c r="S32" s="3"/>
+      <c r="T32" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3">
+        <v>3</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3">
+        <v>8</v>
+      </c>
+      <c r="G33" s="3">
+        <v>2</v>
+      </c>
+      <c r="H33" s="3">
+        <v>5</v>
+      </c>
+      <c r="I33" s="3">
+        <v>4</v>
+      </c>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3">
+        <v>7</v>
+      </c>
+      <c r="O33" s="3">
+        <v>10</v>
+      </c>
+      <c r="P33" s="3">
+        <v>11</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>1</v>
+      </c>
+      <c r="R33" s="3">
+        <v>9</v>
+      </c>
+      <c r="S33" s="3"/>
+      <c r="T33" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3">
+        <v>3</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>8</v>
+      </c>
+      <c r="G34" s="3">
+        <v>2</v>
+      </c>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3">
+        <v>4</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3">
+        <v>7</v>
+      </c>
+      <c r="O34" s="3">
+        <v>10</v>
+      </c>
+      <c r="P34" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>1</v>
+      </c>
+      <c r="R34" s="3">
+        <v>9</v>
+      </c>
+      <c r="S34" s="3">
+        <v>11</v>
+      </c>
+      <c r="T34" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3">
+        <v>12</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3">
+        <v>8</v>
+      </c>
+      <c r="G35" s="3">
+        <v>2</v>
+      </c>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3">
+        <v>7</v>
+      </c>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N35" s="3">
+        <v>14</v>
+      </c>
+      <c r="O35" s="3">
+        <v>10</v>
+      </c>
+      <c r="P35" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>1</v>
+      </c>
+      <c r="R35" s="3">
+        <v>9</v>
+      </c>
+      <c r="S35" s="3">
+        <v>11</v>
+      </c>
+      <c r="T35" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3">
+        <v>2</v>
+      </c>
+      <c r="F36" s="3">
+        <v>8</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3">
+        <v>5</v>
+      </c>
+      <c r="I36" s="3">
+        <v>4</v>
+      </c>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3">
+        <v>7</v>
+      </c>
+      <c r="O36" s="3">
+        <v>10</v>
+      </c>
+      <c r="P36" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>1</v>
+      </c>
+      <c r="R36" s="3">
+        <v>9</v>
+      </c>
+      <c r="S36" s="3">
+        <v>11</v>
+      </c>
+      <c r="T36" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3">
+        <v>12</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2</v>
+      </c>
+      <c r="F37" s="3">
+        <v>8</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3">
+        <v>5</v>
+      </c>
+      <c r="I37" s="3">
+        <v>4</v>
+      </c>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3">
+        <v>14</v>
+      </c>
+      <c r="N37" s="3">
+        <v>7</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P37" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>1</v>
+      </c>
+      <c r="R37" s="3">
+        <v>9</v>
+      </c>
+      <c r="S37" s="3">
+        <v>11</v>
+      </c>
+      <c r="T37" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3">
+        <v>12</v>
+      </c>
+      <c r="E38" s="3">
+        <v>6</v>
+      </c>
+      <c r="F38" s="3">
+        <v>8</v>
+      </c>
+      <c r="G38" s="3">
+        <v>2</v>
+      </c>
+      <c r="H38" s="3">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3">
+        <v>4</v>
+      </c>
+      <c r="N38" s="3">
+        <v>14</v>
+      </c>
+      <c r="O38" s="3">
+        <v>10</v>
+      </c>
+      <c r="P38" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>1</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S38" s="3">
+        <v>11</v>
+      </c>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3">
+        <v>6</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2</v>
+      </c>
+      <c r="H39" s="3">
+        <v>5</v>
+      </c>
+      <c r="I39" s="3">
+        <v>7</v>
+      </c>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3">
+        <v>4</v>
+      </c>
+      <c r="N39" s="3">
+        <v>14</v>
+      </c>
+      <c r="O39" s="3">
+        <v>10</v>
+      </c>
+      <c r="P39" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>1</v>
+      </c>
+      <c r="R39" s="3">
+        <v>9</v>
+      </c>
+      <c r="S39" s="3">
+        <v>11</v>
+      </c>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3">
+        <v>12</v>
+      </c>
+      <c r="E40" s="3">
+        <v>6</v>
+      </c>
+      <c r="F40" s="3">
+        <v>8</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H40" s="3">
+        <v>5</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3">
+        <v>4</v>
+      </c>
+      <c r="N40" s="3">
+        <v>14</v>
+      </c>
+      <c r="O40" s="3">
+        <v>10</v>
+      </c>
+      <c r="P40" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1</v>
+      </c>
+      <c r="R40" s="3">
+        <v>9</v>
+      </c>
+      <c r="S40" s="3">
+        <v>11</v>
+      </c>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3">
+        <v>6</v>
+      </c>
+      <c r="F41" s="3">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H41" s="3">
+        <v>5</v>
+      </c>
+      <c r="I41" s="3">
+        <v>12</v>
+      </c>
+      <c r="J41" s="3">
+        <v>14</v>
+      </c>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3">
+        <v>4</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O41" s="3">
+        <v>10</v>
+      </c>
+      <c r="P41" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>1</v>
+      </c>
+      <c r="R41" s="3">
+        <v>9</v>
+      </c>
+      <c r="S41" s="3">
+        <v>11</v>
+      </c>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3">
+        <v>2</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3">
+        <v>5</v>
+      </c>
+      <c r="I42" s="3">
+        <v>12</v>
+      </c>
+      <c r="J42" s="3">
+        <v>14</v>
+      </c>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3">
+        <v>4</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O42" s="3">
+        <v>10</v>
+      </c>
+      <c r="P42" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>1</v>
+      </c>
+      <c r="R42" s="3">
+        <v>9</v>
+      </c>
+      <c r="S42" s="3">
+        <v>11</v>
+      </c>
+      <c r="T42" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3">
+        <v>2</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3">
+        <v>5</v>
+      </c>
+      <c r="I43" s="3">
+        <v>12</v>
+      </c>
+      <c r="J43" s="3">
+        <v>14</v>
+      </c>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3">
+        <v>4</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O43" s="3">
+        <v>10</v>
+      </c>
+      <c r="P43" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>1</v>
+      </c>
+      <c r="R43" s="3">
+        <v>9</v>
+      </c>
+      <c r="S43" s="3">
+        <v>11</v>
+      </c>
+      <c r="T43" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3">
+        <v>2</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3">
+        <v>5</v>
+      </c>
+      <c r="I44" s="3">
+        <v>7</v>
+      </c>
+      <c r="J44" s="3">
+        <v>12</v>
+      </c>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3">
+        <v>4</v>
+      </c>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3">
+        <v>10</v>
+      </c>
+      <c r="P44" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3">
+        <v>9</v>
+      </c>
+      <c r="S44" s="3">
+        <v>11</v>
+      </c>
+      <c r="T44" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3">
+        <v>2</v>
+      </c>
+      <c r="F45" s="3">
+        <v>8</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3">
+        <v>5</v>
+      </c>
+      <c r="I45" s="3">
+        <v>7</v>
+      </c>
+      <c r="J45" s="3">
+        <v>12</v>
+      </c>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3">
+        <v>4</v>
+      </c>
+      <c r="N45" s="3">
+        <v>14</v>
+      </c>
+      <c r="O45" s="3">
+        <v>10</v>
+      </c>
+      <c r="P45" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="T45" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3">
+        <v>5</v>
+      </c>
+      <c r="I46" s="3">
+        <v>8</v>
+      </c>
+      <c r="J46" s="3">
+        <v>12</v>
+      </c>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3">
+        <v>4</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O46" s="3">
+        <v>10</v>
+      </c>
+      <c r="P46" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3">
+        <v>9</v>
+      </c>
+      <c r="S46" s="3">
+        <v>11</v>
+      </c>
+      <c r="T46" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3">
+        <v>2</v>
+      </c>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3">
+        <v>5</v>
+      </c>
+      <c r="I47" s="3">
+        <v>8</v>
+      </c>
+      <c r="J47" s="3">
+        <v>12</v>
+      </c>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3">
+        <v>4</v>
+      </c>
+      <c r="N47" s="3">
+        <v>7</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P47" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>1</v>
+      </c>
+      <c r="R47" s="3">
+        <v>9</v>
+      </c>
+      <c r="S47" s="3">
+        <v>11</v>
+      </c>
+      <c r="T47" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3">
+        <v>12</v>
+      </c>
+      <c r="E48" s="3">
+        <v>2</v>
+      </c>
+      <c r="F48" s="3">
+        <v>14</v>
+      </c>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3">
+        <v>5</v>
+      </c>
+      <c r="I48" s="3">
+        <v>8</v>
+      </c>
+      <c r="J48" s="3">
+        <v>10</v>
+      </c>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3">
+        <v>4</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>1</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S48" s="3">
+        <v>11</v>
+      </c>
+      <c r="T48" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3">
+        <v>5</v>
+      </c>
+      <c r="I49" s="3">
+        <v>8</v>
+      </c>
+      <c r="J49" s="3">
+        <v>10</v>
+      </c>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3">
+        <v>4</v>
+      </c>
+      <c r="N49" s="3">
+        <v>7</v>
+      </c>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>1</v>
+      </c>
+      <c r="R49" s="3">
+        <v>9</v>
+      </c>
+      <c r="S49" s="3">
+        <v>11</v>
+      </c>
+      <c r="T49" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3">
+        <v>12</v>
+      </c>
+      <c r="E50" s="3">
+        <v>2</v>
+      </c>
+      <c r="F50" s="3">
+        <v>14</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I50" s="3">
+        <v>8</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3">
+        <v>4</v>
+      </c>
+      <c r="N50" s="3">
+        <v>7</v>
+      </c>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>1</v>
+      </c>
+      <c r="R50" s="3">
+        <v>9</v>
+      </c>
+      <c r="S50" s="3">
+        <v>11</v>
+      </c>
+      <c r="T50" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3">
+        <v>14</v>
+      </c>
+      <c r="E51" s="3">
+        <v>2</v>
+      </c>
+      <c r="F51" s="3">
+        <v>12</v>
+      </c>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I51" s="3">
+        <v>8</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3">
+        <v>4</v>
+      </c>
+      <c r="N51" s="3">
+        <v>7</v>
+      </c>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>1</v>
+      </c>
+      <c r="R51" s="3">
+        <v>9</v>
+      </c>
+      <c r="S51" s="3">
+        <v>11</v>
+      </c>
+      <c r="T51" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3">
+        <v>12</v>
+      </c>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>8</v>
+      </c>
+      <c r="G52" s="3">
+        <v>2</v>
+      </c>
+      <c r="H52" s="3">
+        <v>5</v>
+      </c>
+      <c r="I52" s="3">
+        <v>14</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3">
+        <v>4</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>1</v>
+      </c>
+      <c r="R52" s="3">
+        <v>9</v>
+      </c>
+      <c r="S52" s="3">
+        <v>11</v>
+      </c>
+      <c r="T52" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3">
+        <v>12</v>
+      </c>
+      <c r="E53" s="3">
+        <v>5</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G53" s="3">
+        <v>2</v>
+      </c>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3">
+        <v>10</v>
+      </c>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3">
+        <v>4</v>
+      </c>
+      <c r="N53" s="3">
+        <v>7</v>
+      </c>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>1</v>
+      </c>
+      <c r="R53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S53" s="3">
+        <v>11</v>
+      </c>
+      <c r="T53" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3">
+        <v>10</v>
+      </c>
+      <c r="E54" s="3">
+        <v>5</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G54" s="3">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3">
+        <v>14</v>
+      </c>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3">
+        <v>4</v>
+      </c>
+      <c r="N54" s="3">
+        <v>7</v>
+      </c>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>1</v>
+      </c>
+      <c r="R54" s="3">
+        <v>9</v>
+      </c>
+      <c r="S54" s="3">
+        <v>11</v>
+      </c>
+      <c r="T54" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3">
+        <v>5</v>
+      </c>
+      <c r="I55" s="3">
+        <v>8</v>
+      </c>
+      <c r="J55" s="3">
+        <v>12</v>
+      </c>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3">
+        <v>4</v>
+      </c>
+      <c r="N55" s="3">
+        <v>7</v>
+      </c>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q55" s="3">
+        <v>1</v>
+      </c>
+      <c r="R55" s="3">
+        <v>9</v>
+      </c>
+      <c r="S55" s="3">
+        <v>11</v>
+      </c>
+      <c r="T55" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3">
+        <v>2</v>
+      </c>
+      <c r="H56" s="3">
+        <v>5</v>
+      </c>
+      <c r="I56" s="3">
+        <v>8</v>
+      </c>
+      <c r="J56" s="3">
+        <v>12</v>
+      </c>
+      <c r="K56" s="3">
+        <v>14</v>
+      </c>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3">
+        <v>4</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>1</v>
+      </c>
+      <c r="R56" s="3">
+        <v>9</v>
+      </c>
+      <c r="S56" s="3">
+        <v>11</v>
+      </c>
+      <c r="T56" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3">
+        <v>10</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3">
+        <v>2</v>
+      </c>
+      <c r="H57" s="3">
+        <v>5</v>
+      </c>
+      <c r="I57" s="3">
+        <v>8</v>
+      </c>
+      <c r="J57" s="3">
+        <v>12</v>
+      </c>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3">
+        <v>4</v>
+      </c>
+      <c r="N57" s="3">
+        <v>7</v>
+      </c>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>1</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S57" s="3">
+        <v>11</v>
+      </c>
+      <c r="T57" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3">
+        <v>14</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3">
+        <v>10</v>
+      </c>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3">
+        <v>2</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="3">
+        <v>8</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K58" s="3">
+        <v>12</v>
+      </c>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3">
+        <v>4</v>
+      </c>
+      <c r="N58" s="3">
+        <v>7</v>
+      </c>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>1</v>
+      </c>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3">
+        <v>11</v>
+      </c>
+      <c r="T58" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3">
+        <v>10</v>
+      </c>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3">
+        <v>4</v>
+      </c>
+      <c r="G59" s="3">
+        <v>2</v>
+      </c>
+      <c r="H59" s="3">
+        <v>5</v>
+      </c>
+      <c r="I59" s="3">
+        <v>8</v>
+      </c>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3">
+        <v>14</v>
+      </c>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3">
+        <v>7</v>
+      </c>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>1</v>
+      </c>
+      <c r="R59" s="3">
+        <v>9</v>
+      </c>
+      <c r="S59" s="3">
+        <v>11</v>
+      </c>
+      <c r="T59" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3">
+        <v>10</v>
+      </c>
+      <c r="E60" s="3">
+        <v>12</v>
+      </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3">
+        <v>2</v>
+      </c>
+      <c r="H60" s="3">
+        <v>5</v>
+      </c>
+      <c r="I60" s="3">
+        <v>4</v>
+      </c>
+      <c r="J60" s="3">
+        <v>14</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3">
+        <v>1</v>
+      </c>
+      <c r="R60" s="3">
+        <v>9</v>
+      </c>
+      <c r="S60" s="3">
+        <v>11</v>
+      </c>
+      <c r="T60" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3">
+        <v>3</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3">
+        <v>10</v>
+      </c>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3">
+        <v>2</v>
+      </c>
+      <c r="H61" s="3">
+        <v>5</v>
+      </c>
+      <c r="I61" s="3">
+        <v>8</v>
+      </c>
+      <c r="J61" s="3">
+        <v>12</v>
+      </c>
+      <c r="K61" s="3">
+        <v>14</v>
+      </c>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N61" s="3">
+        <v>7</v>
+      </c>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3">
+        <v>1</v>
+      </c>
+      <c r="R61" s="3">
+        <v>9</v>
+      </c>
+      <c r="S61" s="3">
+        <v>11</v>
+      </c>
+      <c r="T61" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3">
+        <v>3</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3">
+        <v>10</v>
+      </c>
+      <c r="E62" s="3">
+        <v>6</v>
+      </c>
+      <c r="F62" s="3">
+        <v>14</v>
+      </c>
+      <c r="G62" s="3">
+        <v>2</v>
+      </c>
+      <c r="H62" s="3">
+        <v>5</v>
+      </c>
+      <c r="I62" s="3">
+        <v>4</v>
+      </c>
+      <c r="J62" s="3">
+        <v>12</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3">
+        <v>7</v>
+      </c>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3">
+        <v>1</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S62" s="3">
+        <v>11</v>
+      </c>
+      <c r="T62" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEC80A8-202C-9946-8EBB-EFD49AAE7C1A}">
   <dimension ref="A1:W60"/>
   <sheetViews>
@@ -2974,23 +5913,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BAF2C6-109D-1143-8A73-37780FE37E32}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9AD14E-5C41-B640-841F-A02FBCF76B8F}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:W60"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 1945-46 goals and app, added examples dir,
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7DE7333-8E3A-AA40-A486-765B466E7F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F80A8BD-310D-4E4F-AB24-ECABC3695FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="1989-90" sheetId="17" r:id="rId1"/>
-    <sheet name="1990-91" sheetId="16" r:id="rId2"/>
-    <sheet name="1991-92" sheetId="7" r:id="rId3"/>
-    <sheet name="1992-93" sheetId="11" r:id="rId4"/>
-    <sheet name="1993-94" sheetId="14" r:id="rId5"/>
-    <sheet name="1994-95" sheetId="1" r:id="rId6"/>
-    <sheet name="1995-96" sheetId="4" r:id="rId7"/>
+    <sheet name="1945-46" sheetId="18" r:id="rId1"/>
+    <sheet name="1989-90" sheetId="17" r:id="rId2"/>
+    <sheet name="1990-91" sheetId="16" r:id="rId3"/>
+    <sheet name="1991-92" sheetId="7" r:id="rId4"/>
+    <sheet name="1992-93" sheetId="11" r:id="rId5"/>
+    <sheet name="1993-94" sheetId="14" r:id="rId6"/>
+    <sheet name="1994-95" sheetId="1" r:id="rId7"/>
+    <sheet name="1995-96" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="106">
   <si>
     <t>11+</t>
   </si>
@@ -295,12 +296,78 @@
   <si>
     <t>4•</t>
   </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Ashcroft</t>
+  </si>
+  <si>
+    <t>Atkinson</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>Bridges</t>
+  </si>
+  <si>
+    <t>Gould</t>
+  </si>
+  <si>
+    <t>Grant</t>
+  </si>
+  <si>
+    <t>Harlock</t>
+  </si>
+  <si>
+    <t>Hodgson L</t>
+  </si>
+  <si>
+    <t>Hornby</t>
+  </si>
+  <si>
+    <t>Jones TB</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>Lloyd</t>
+  </si>
+  <si>
+    <t>Payne AC</t>
+  </si>
+  <si>
+    <t>Phiipotts</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Richards</t>
+  </si>
+  <si>
+    <t>Riley</t>
+  </si>
+  <si>
+    <t>Rosenthal</t>
+  </si>
+  <si>
+    <t>Steele</t>
+  </si>
+  <si>
+    <t>Williamson S</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -327,6 +394,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -356,6 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,11 +743,370 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA77E507-ADE4-EC47-A9C7-E6FD7EAE7A4E}">
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5">
+        <v>3</v>
+      </c>
+      <c r="K2" s="5">
+        <v>11</v>
+      </c>
+      <c r="L2" s="5">
+        <v>8</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5">
+        <v>5</v>
+      </c>
+      <c r="S2" s="5">
+        <v>1</v>
+      </c>
+      <c r="T2" s="5">
+        <v>10</v>
+      </c>
+      <c r="U2" s="5">
+        <v>4</v>
+      </c>
+      <c r="V2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5">
+        <v>3</v>
+      </c>
+      <c r="K3" s="5">
+        <v>11</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5">
+        <v>5</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5">
+        <v>8</v>
+      </c>
+      <c r="U3" s="5">
+        <v>4</v>
+      </c>
+      <c r="V3" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>3</v>
+      </c>
+      <c r="K4" s="5">
+        <v>11</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5">
+        <v>5</v>
+      </c>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5">
+        <v>8</v>
+      </c>
+      <c r="U4" s="5">
+        <v>4</v>
+      </c>
+      <c r="V4" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <v>3</v>
+      </c>
+      <c r="K5" s="5">
+        <v>11</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5">
+        <v>1</v>
+      </c>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5">
+        <v>7</v>
+      </c>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5">
+        <v>5</v>
+      </c>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5">
+        <v>8</v>
+      </c>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>9</v>
+      </c>
+      <c r="G6" s="5">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5">
+        <v>2</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3</v>
+      </c>
+      <c r="K6" s="5">
+        <v>11</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5">
+        <v>1</v>
+      </c>
+      <c r="N6" s="5">
+        <v>4</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5">
+        <v>8</v>
+      </c>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <v>7</v>
+      </c>
+      <c r="I7" s="5">
+        <v>2</v>
+      </c>
+      <c r="J7" s="5">
+        <v>3</v>
+      </c>
+      <c r="K7" s="5">
+        <v>11</v>
+      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5">
+        <v>8</v>
+      </c>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0C9159-3439-D04D-A570-3940686A82F2}">
   <dimension ref="A1:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4679,7 +5112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B1DCE2-83C0-7043-83EC-E3BF8EDF97DC}">
   <dimension ref="A1:T62"/>
   <sheetViews>
@@ -7594,7 +8027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEC80A8-202C-9946-8EBB-EFD49AAE7C1A}">
   <dimension ref="A1:W60"/>
   <sheetViews>
@@ -9946,7 +10379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9AD14E-5C41-B640-841F-A02FBCF76B8F}">
   <dimension ref="A1:W60"/>
   <sheetViews>
@@ -12256,7 +12689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B21AD3B-5CFD-9E48-9F5E-34B590DA3414}">
   <dimension ref="A1:X60"/>
   <sheetViews>
@@ -14572,7 +15005,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A364B2D-8A97-644E-815B-092AA8749711}">
   <dimension ref="A1:V60"/>
   <sheetViews>
@@ -16927,7 +17360,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AACCB4-B063-5940-B7D8-989E5CF6472C}">
   <dimension ref="A1:AC52"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed error in excel sheets
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B6406BB4-08F0-F340-99CD-9148B634CC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7754C1A2-8E16-494D-9613-3C5937A23E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30180" windowHeight="28800" activeTab="4" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="1921-22" sheetId="19" r:id="rId1"/>
@@ -14807,7 +14807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0918A408-A8FE-FD46-B853-09BED4383EC7}">
   <dimension ref="A1:Y53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -26775,8 +26775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9AD14E-5C41-B640-841F-A02FBCF76B8F}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:W60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26880,7 +26880,7 @@
       <c r="S2">
         <v>1</v>
       </c>
-      <c r="U2">
+      <c r="T2">
         <v>3</v>
       </c>
       <c r="V2">
@@ -26921,7 +26921,7 @@
       <c r="S3">
         <v>1</v>
       </c>
-      <c r="U3">
+      <c r="T3">
         <v>3</v>
       </c>
       <c r="V3">
@@ -26959,7 +26959,7 @@
       <c r="S4">
         <v>1</v>
       </c>
-      <c r="U4">
+      <c r="T4">
         <v>3</v>
       </c>
       <c r="V4">
@@ -27000,7 +27000,7 @@
       <c r="S5">
         <v>1</v>
       </c>
-      <c r="U5">
+      <c r="T5">
         <v>3</v>
       </c>
       <c r="V5">
@@ -27038,7 +27038,7 @@
       <c r="S6">
         <v>1</v>
       </c>
-      <c r="U6">
+      <c r="T6">
         <v>3</v>
       </c>
       <c r="V6">
@@ -27076,7 +27076,7 @@
       <c r="S7">
         <v>1</v>
       </c>
-      <c r="U7">
+      <c r="T7">
         <v>3</v>
       </c>
       <c r="V7" t="s">
@@ -27111,7 +27111,7 @@
       <c r="S8">
         <v>1</v>
       </c>
-      <c r="U8">
+      <c r="T8">
         <v>3</v>
       </c>
       <c r="W8">
@@ -27152,7 +27152,7 @@
       <c r="S9">
         <v>1</v>
       </c>
-      <c r="U9" t="s">
+      <c r="T9" t="s">
         <v>12</v>
       </c>
       <c r="W9">

</xml_diff>

<commit_message>
fixed issues with 92-3
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7754C1A2-8E16-494D-9613-3C5937A23E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F20A0F2-1266-4A4F-B33E-6952F17EE402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="8" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="1921-22" sheetId="19" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="150">
   <si>
     <t>11+</t>
   </si>
@@ -263,9 +263,6 @@
   </si>
   <si>
     <t>Coyne T</t>
-  </si>
-  <si>
-    <t>trons</t>
   </si>
   <si>
     <t>Jones M</t>
@@ -899,97 +896,97 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -2401,7 +2398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B21AD3B-5CFD-9E48-9F5E-34B590DA3414}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X60"/>
     </sheetView>
   </sheetViews>
@@ -2436,7 +2433,7 @@
         <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>31</v>
@@ -2641,7 +2638,7 @@
         <v>4</v>
       </c>
       <c r="K6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L6">
         <v>9</v>
@@ -9202,49 +9199,49 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -9454,43 +9451,43 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>134</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>63</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>34</v>
@@ -9505,22 +9502,22 @@
         <v>37</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>138</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -12042,7 +12039,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>60</v>
@@ -12063,10 +12060,10 @@
         <v>66</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>34</v>
@@ -12081,13 +12078,13 @@
         <v>37</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>69</v>
@@ -12099,7 +12096,7 @@
         <v>65</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -13814,7 +13811,7 @@
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H39" s="4">
         <v>3</v>
@@ -13906,7 +13903,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H41" s="4">
         <v>3</v>
@@ -14815,25 +14812,25 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>147</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>62</v>
@@ -14851,10 +14848,10 @@
         <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>34</v>
@@ -14869,25 +14866,25 @@
         <v>37</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
@@ -17505,13 +17502,13 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>27</v>
@@ -17535,7 +17532,7 @@
         <v>66</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>68</v>
@@ -17553,7 +17550,7 @@
         <v>39</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>69</v>
@@ -17567,16 +17564,16 @@
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B2" s="4">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="4">
         <v>8</v>
@@ -17588,19 +17585,19 @@
         <v>5</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I2" s="4">
         <v>12</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="4">
         <v>3</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M2" s="4">
         <v>7</v>
@@ -17609,13 +17606,13 @@
         <v>10</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P2" s="4">
         <v>1</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>14</v>
@@ -17629,16 +17626,16 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="4">
         <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E3" s="4">
         <v>8</v>
@@ -17650,19 +17647,19 @@
         <v>5</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I3" s="4">
         <v>9</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K3" s="4">
         <v>3</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M3" s="4">
         <v>7</v>
@@ -17671,16 +17668,16 @@
         <v>10</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P3" s="4">
         <v>1</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S3" s="4">
         <v>11</v>
@@ -17695,10 +17692,10 @@
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="4">
         <v>8</v>
@@ -17710,19 +17707,19 @@
         <v>5</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I4" s="4">
         <v>9</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K4" s="4">
         <v>3</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M4" s="4">
         <v>7</v>
@@ -17731,16 +17728,16 @@
         <v>10</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P4" s="4">
         <v>1</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S4" s="4">
         <v>11</v>
@@ -17758,7 +17755,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="4">
         <v>8</v>
@@ -17770,7 +17767,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I5" s="4">
         <v>9</v>
@@ -17782,7 +17779,7 @@
         <v>3</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>17</v>
@@ -17791,16 +17788,16 @@
         <v>10</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P5" s="4">
         <v>1</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S5" s="4">
         <v>11</v>
@@ -17818,7 +17815,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E6" s="4">
         <v>8</v>
@@ -17830,19 +17827,19 @@
         <v>4</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I6" s="4">
         <v>9</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K6" s="4">
         <v>3</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M6" s="4">
         <v>7</v>
@@ -17851,16 +17848,16 @@
         <v>10</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P6" s="4">
         <v>1</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S6" s="4">
         <v>11</v>
@@ -17878,7 +17875,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="4">
         <v>8</v>
@@ -17890,19 +17887,19 @@
         <v>5</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I7" s="4">
         <v>9</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K7" s="4">
         <v>3</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>17</v>
@@ -17911,16 +17908,16 @@
         <v>10</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P7" s="4">
         <v>1</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S7" s="4">
         <v>11</v>
@@ -17938,7 +17935,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E8" s="4">
         <v>8</v>
@@ -17950,7 +17947,7 @@
         <v>4</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" s="4">
         <v>9</v>
@@ -17962,7 +17959,7 @@
         <v>3</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M8" s="4">
         <v>7</v>
@@ -17971,16 +17968,16 @@
         <v>10</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P8" s="4">
         <v>1</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S8" s="4">
         <v>11</v>
@@ -17995,7 +17992,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>13</v>
@@ -18010,7 +18007,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="4">
         <v>9</v>
@@ -18022,7 +18019,7 @@
         <v>3</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>17</v>
@@ -18031,13 +18028,13 @@
         <v>10</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P9" s="4">
         <v>1</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R9" s="4">
         <v>12</v>
@@ -18046,7 +18043,7 @@
         <v>11</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -18055,10 +18052,10 @@
         <v>14</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="4">
         <v>8</v>
@@ -18070,7 +18067,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I10" s="4">
         <v>9</v>
@@ -18082,7 +18079,7 @@
         <v>3</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M10" s="4">
         <v>7</v>
@@ -18091,16 +18088,16 @@
         <v>10</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P10" s="4">
         <v>1</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S10" s="4">
         <v>11</v>
@@ -18115,10 +18112,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E11" s="4">
         <v>8</v>
@@ -18130,7 +18127,7 @@
         <v>5</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="4">
         <v>9</v>
@@ -18142,7 +18139,7 @@
         <v>3</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>17</v>
@@ -18151,13 +18148,13 @@
         <v>10</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P11" s="4">
         <v>1</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R11" s="4">
         <v>12</v>
@@ -18175,10 +18172,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="4">
         <v>8</v>
@@ -18190,7 +18187,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I12" s="4">
         <v>9</v>
@@ -18202,7 +18199,7 @@
         <v>3</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M12" s="4">
         <v>7</v>
@@ -18211,16 +18208,16 @@
         <v>10</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P12" s="4">
         <v>1</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S12" s="4">
         <v>11</v>
@@ -18235,10 +18232,10 @@
         <v>12</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E13" s="4">
         <v>8</v>
@@ -18250,7 +18247,7 @@
         <v>5</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I13" s="4">
         <v>9</v>
@@ -18262,7 +18259,7 @@
         <v>3</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>5</v>
@@ -18271,13 +18268,13 @@
         <v>10</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P13" s="4">
         <v>1</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R13" s="4">
         <v>14</v>
@@ -18292,13 +18289,13 @@
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E14" s="4">
         <v>8</v>
@@ -18310,7 +18307,7 @@
         <v>5</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I14" s="4">
         <v>9</v>
@@ -18322,7 +18319,7 @@
         <v>3</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M14" s="4">
         <v>7</v>
@@ -18331,16 +18328,16 @@
         <v>10</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P14" s="4">
         <v>1</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S14" s="4">
         <v>11</v>
@@ -18355,10 +18352,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E15" s="4">
         <v>8</v>
@@ -18370,7 +18367,7 @@
         <v>5</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I15" s="4">
         <v>9</v>
@@ -18382,7 +18379,7 @@
         <v>10</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M15" s="4">
         <v>7</v>
@@ -18391,16 +18388,16 @@
         <v>10</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P15" s="4">
         <v>1</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S15" s="4">
         <v>11</v>
@@ -18415,10 +18412,10 @@
         <v>12</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E16" s="4">
         <v>8</v>
@@ -18430,7 +18427,7 @@
         <v>5</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I16" s="4">
         <v>9</v>
@@ -18442,7 +18439,7 @@
         <v>3</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M16" s="4">
         <v>7</v>
@@ -18451,13 +18448,13 @@
         <v>10</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P16" s="4">
         <v>1</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R16" s="4">
         <v>14</v>
@@ -18475,7 +18472,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D17" s="4">
         <v>6</v>
@@ -18490,7 +18487,7 @@
         <v>5</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>11</v>
@@ -18502,7 +18499,7 @@
         <v>3</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M17" s="4">
         <v>7</v>
@@ -18511,13 +18508,13 @@
         <v>10</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P17" s="4">
         <v>1</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R17" s="4">
         <v>14</v>
@@ -18526,7 +18523,7 @@
         <v>11</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
@@ -18538,7 +18535,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E18" s="4">
         <v>8</v>
@@ -18550,7 +18547,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I18" s="4">
         <v>9</v>
@@ -18562,7 +18559,7 @@
         <v>3</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>17</v>
@@ -18571,13 +18568,13 @@
         <v>10</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P18" s="4">
         <v>1</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R18" s="4">
         <v>6</v>
@@ -18586,7 +18583,7 @@
         <v>11</v>
       </c>
       <c r="T18" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -18595,10 +18592,10 @@
         <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="4">
         <v>8</v>
@@ -18610,19 +18607,19 @@
         <v>5</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I19" s="4">
         <v>9</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K19" s="4">
         <v>3</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M19" s="4">
         <v>7</v>
@@ -18631,16 +18628,16 @@
         <v>10</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P19" s="4">
         <v>1</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S19" s="4">
         <v>11</v>
@@ -18655,10 +18652,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E20" s="4">
         <v>8</v>
@@ -18670,19 +18667,19 @@
         <v>5</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I20" s="4">
         <v>9</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>12</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M20" s="4">
         <v>7</v>
@@ -18691,13 +18688,13 @@
         <v>10</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P20" s="4">
         <v>1</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R20" s="4">
         <v>14</v>
@@ -18715,7 +18712,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="4">
         <v>6</v>
@@ -18730,19 +18727,19 @@
         <v>5</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K21" s="4">
         <v>3</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M21" s="4">
         <v>7</v>
@@ -18757,16 +18754,16 @@
         <v>1</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R21" s="4">
         <v>9</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
@@ -18781,7 +18778,7 @@
         <v>6</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F22" s="4">
         <v>2</v>
@@ -18790,7 +18787,7 @@
         <v>5</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I22" s="4">
         <v>12</v>
@@ -18802,7 +18799,7 @@
         <v>12</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>17</v>
@@ -18817,16 +18814,16 @@
         <v>1</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R22" s="4">
         <v>9</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
@@ -18835,10 +18832,10 @@
         <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>21</v>
@@ -18850,10 +18847,10 @@
         <v>5</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J23" s="4">
         <v>12</v>
@@ -18862,7 +18859,7 @@
         <v>3</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M23" s="4">
         <v>7</v>
@@ -18877,13 +18874,13 @@
         <v>1</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R23" s="4">
         <v>9</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T23" s="4">
         <v>6</v>
@@ -18895,10 +18892,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E24" s="4">
         <v>8</v>
@@ -18910,19 +18907,19 @@
         <v>5</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I24" s="4">
         <v>14</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M24" s="4" t="s">
         <v>5</v>
@@ -18943,7 +18940,7 @@
         <v>9</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T24" s="4">
         <v>6</v>
@@ -18955,10 +18952,10 @@
         <v>20</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E25" s="4">
         <v>8</v>
@@ -18970,7 +18967,7 @@
         <v>5</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I25" s="4">
         <v>14</v>
@@ -18979,10 +18976,10 @@
         <v>12</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>5</v>
@@ -19003,7 +19000,7 @@
         <v>9</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T25" s="4">
         <v>6</v>
@@ -19012,13 +19009,13 @@
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="4">
         <v>14</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E26" s="4">
         <v>8</v>
@@ -19030,7 +19027,7 @@
         <v>5</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I26" s="4">
         <v>7</v>
@@ -19039,13 +19036,13 @@
         <v>6</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N26" s="4">
         <v>10</v>
@@ -19078,7 +19075,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E27" s="4">
         <v>8</v>
@@ -19090,7 +19087,7 @@
         <v>5</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I27" s="4" t="s">
         <v>17</v>
@@ -19099,13 +19096,13 @@
         <v>6</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N27" s="4">
         <v>10</v>
@@ -19123,7 +19120,7 @@
         <v>9</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T27" s="4">
         <v>6</v>
@@ -19138,7 +19135,7 @@
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E28" s="4">
         <v>8</v>
@@ -19159,13 +19156,13 @@
         <v>6</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N28" s="4">
         <v>10</v>
@@ -19180,10 +19177,10 @@
         <v>3</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T28" s="4">
         <v>6</v>
@@ -19192,10 +19189,10 @@
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="4">
         <v>14</v>
@@ -19210,7 +19207,7 @@
         <v>5</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I29" s="4">
         <v>7</v>
@@ -19222,22 +19219,22 @@
         <v>3</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N29" s="4">
         <v>10</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P29" s="4">
         <v>1</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R29" s="4">
         <v>9</v>
@@ -19252,13 +19249,13 @@
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C30" s="4">
         <v>12</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E30" s="4">
         <v>8</v>
@@ -19270,7 +19267,7 @@
         <v>5</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I30" s="4">
         <v>7</v>
@@ -19282,22 +19279,22 @@
         <v>3</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N30" s="4">
         <v>10</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P30" s="4">
         <v>1</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R30" s="4">
         <v>9</v>
@@ -19318,7 +19315,7 @@
         <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>21</v>
@@ -19330,7 +19327,7 @@
         <v>5</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I31" s="4">
         <v>12</v>
@@ -19342,28 +19339,28 @@
         <v>3</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N31" s="4">
         <v>10</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P31" s="4">
         <v>1</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R31" s="4">
         <v>9</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="T31" s="4">
         <v>6</v>
@@ -19378,7 +19375,7 @@
         <v>17</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>8</v>
@@ -19390,7 +19387,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I32" s="4">
         <v>12</v>
@@ -19402,22 +19399,22 @@
         <v>3</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N32" s="4">
         <v>10</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P32" s="4">
         <v>1</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R32" s="4">
         <v>9</v>
@@ -19432,13 +19429,13 @@
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E33" s="4">
         <v>8</v>
@@ -19450,13 +19447,13 @@
         <v>4</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I33" s="4">
         <v>9</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K33" s="4">
         <v>3</v>
@@ -19471,13 +19468,13 @@
         <v>10</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P33" s="4">
         <v>1</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R33" s="4">
         <v>12</v>
@@ -19492,13 +19489,13 @@
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E34" s="4">
         <v>8</v>
@@ -19510,13 +19507,13 @@
         <v>5</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I34" s="4">
         <v>9</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K34" s="4">
         <v>3</v>
@@ -19531,16 +19528,16 @@
         <v>10</v>
       </c>
       <c r="O34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P34" s="4">
         <v>1</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R34" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="S34" s="4">
         <v>11</v>
@@ -19552,13 +19549,13 @@
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E35" s="4">
         <v>8</v>
@@ -19570,13 +19567,13 @@
         <v>5</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I35" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K35" s="4">
         <v>3</v>
@@ -19591,13 +19588,13 @@
         <v>10</v>
       </c>
       <c r="O35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P35" s="4">
         <v>1</v>
       </c>
       <c r="Q35" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R35" s="4">
         <v>12</v>
@@ -19615,10 +19612,10 @@
         <v>14</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>8</v>
@@ -19630,13 +19627,13 @@
         <v>5</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I36" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K36" s="4">
         <v>3</v>
@@ -19651,13 +19648,13 @@
         <v>10</v>
       </c>
       <c r="O36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P36" s="4">
         <v>1</v>
       </c>
       <c r="Q36" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R36" s="4">
         <v>12</v>
@@ -19672,13 +19669,13 @@
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E37" s="4">
         <v>8</v>
@@ -19690,13 +19687,13 @@
         <v>5</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K37" s="4">
         <v>3</v>
@@ -19711,13 +19708,13 @@
         <v>10</v>
       </c>
       <c r="O37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P37" s="4">
         <v>1</v>
       </c>
       <c r="Q37" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R37" s="4">
         <v>9</v>
@@ -19735,10 +19732,10 @@
         <v>12</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E38" s="4" t="s">
         <v>21</v>
@@ -19753,10 +19750,10 @@
         <v>14</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K38" s="4">
         <v>3</v>
@@ -19771,13 +19768,13 @@
         <v>10</v>
       </c>
       <c r="O38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P38" s="4">
         <v>1</v>
       </c>
       <c r="Q38" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R38" s="4">
         <v>9</v>
@@ -19795,10 +19792,10 @@
         <v>12</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>21</v>
@@ -19810,13 +19807,13 @@
         <v>5</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K39" s="4">
         <v>3</v>
@@ -19831,13 +19828,13 @@
         <v>10</v>
       </c>
       <c r="O39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P39" s="4">
         <v>1</v>
       </c>
       <c r="Q39" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R39" s="4">
         <v>9</v>
@@ -19852,13 +19849,13 @@
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="4"/>
       <c r="B40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="4">
         <v>8</v>
@@ -19870,13 +19867,13 @@
         <v>5</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I40" s="4">
         <v>14</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K40" s="4">
         <v>3</v>
@@ -19891,13 +19888,13 @@
         <v>10</v>
       </c>
       <c r="O40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P40" s="4">
         <v>1</v>
       </c>
       <c r="Q40" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R40" s="4">
         <v>9</v>
@@ -19912,13 +19909,13 @@
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="4"/>
       <c r="B41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" s="4">
         <v>8</v>
@@ -19930,13 +19927,13 @@
         <v>5</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I41" s="4">
         <v>7</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K41" s="4">
         <v>3</v>
@@ -19945,19 +19942,19 @@
         <v>4</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N41" s="4">
         <v>10</v>
       </c>
       <c r="O41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P41" s="4">
         <v>1</v>
       </c>
       <c r="Q41" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R41" s="4">
         <v>9</v>
@@ -19975,10 +19972,10 @@
         <v>12</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42" s="4">
         <v>8</v>
@@ -19990,13 +19987,13 @@
         <v>4</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I42" s="4">
         <v>7</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K42" s="4">
         <v>3</v>
@@ -20005,19 +20002,19 @@
         <v>4</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N42" s="4">
         <v>10</v>
       </c>
       <c r="O42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P42" s="4">
         <v>1</v>
       </c>
       <c r="Q42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R42" s="4">
         <v>9</v>
@@ -20032,31 +20029,31 @@
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="4"/>
       <c r="B43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43" s="4">
         <v>8</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" s="4">
         <v>5</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I43" s="4">
         <v>7</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K43" s="4">
         <v>3</v>
@@ -20065,7 +20062,7 @@
         <v>4</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N43" s="4">
         <v>10</v>
@@ -20077,7 +20074,7 @@
         <v>1</v>
       </c>
       <c r="Q43" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R43" s="4">
         <v>9</v>
@@ -20092,25 +20089,25 @@
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="4"/>
       <c r="B44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E44" s="4">
         <v>8</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G44" s="4">
         <v>5</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I44" s="4">
         <v>7</v>
@@ -20125,7 +20122,7 @@
         <v>4</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N44" s="4">
         <v>10</v>
@@ -20137,7 +20134,7 @@
         <v>1</v>
       </c>
       <c r="Q44" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R44" s="4">
         <v>9</v>
@@ -20155,10 +20152,10 @@
         <v>4</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" s="4">
         <v>8</v>
@@ -20170,7 +20167,7 @@
         <v>5</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I45" s="4">
         <v>7</v>
@@ -20182,22 +20179,22 @@
         <v>3</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="O45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P45" s="4">
         <v>1</v>
       </c>
       <c r="Q45" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R45" s="4">
         <v>9</v>
@@ -20215,10 +20212,10 @@
         <v>4</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E46" s="4">
         <v>8</v>
@@ -20230,7 +20227,7 @@
         <v>5</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I46" s="4">
         <v>7</v>
@@ -20242,22 +20239,22 @@
         <v>10</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N46" s="4">
         <v>10</v>
       </c>
       <c r="O46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P46" s="4">
         <v>1</v>
       </c>
       <c r="Q46" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R46" s="4">
         <v>9</v>
@@ -20275,55 +20272,55 @@
         <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47" s="4">
+        <v>8</v>
+      </c>
+      <c r="F47" s="4">
+        <v>2</v>
+      </c>
+      <c r="G47" s="4">
+        <v>5</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I47" s="4">
+        <v>7</v>
+      </c>
+      <c r="J47" s="4">
+        <v>12</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N47" s="4">
+        <v>10</v>
+      </c>
+      <c r="O47" s="4">
+        <v>3</v>
+      </c>
+      <c r="P47" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="R47" s="4">
+        <v>9</v>
+      </c>
+      <c r="S47" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E47" s="4">
-        <v>8</v>
-      </c>
-      <c r="F47" s="4">
-        <v>2</v>
-      </c>
-      <c r="G47" s="4">
-        <v>5</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="I47" s="4">
-        <v>7</v>
-      </c>
-      <c r="J47" s="4">
-        <v>12</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N47" s="4">
-        <v>10</v>
-      </c>
-      <c r="O47" s="4">
-        <v>3</v>
-      </c>
-      <c r="P47" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q47" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="R47" s="4">
-        <v>9</v>
-      </c>
-      <c r="S47" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="T47" s="4">
         <v>6</v>
@@ -20335,10 +20332,10 @@
         <v>12</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>8</v>
@@ -20350,16 +20347,16 @@
         <v>5</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I48" s="4">
         <v>7</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L48" s="4">
         <v>4</v>
@@ -20377,7 +20374,7 @@
         <v>1</v>
       </c>
       <c r="Q48" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R48" s="4">
         <v>9</v>
@@ -20395,7 +20392,7 @@
         <v>12</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D49" s="4">
         <v>6</v>
@@ -20410,22 +20407,22 @@
         <v>5</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I49" s="4">
         <v>7</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L49" s="4">
         <v>4</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N49" s="4">
         <v>10</v>
@@ -20437,7 +20434,7 @@
         <v>1</v>
       </c>
       <c r="Q49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R49" s="4">
         <v>9</v>
@@ -20446,16 +20443,16 @@
         <v>11</v>
       </c>
       <c r="T49" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D50" s="4">
         <v>6</v>
@@ -20470,22 +20467,22 @@
         <v>5</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I50" s="4">
         <v>7</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L50" s="4">
         <v>4</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N50" s="4">
         <v>10</v>
@@ -20497,7 +20494,7 @@
         <v>1</v>
       </c>
       <c r="Q50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R50" s="4">
         <v>9</v>
@@ -20506,19 +20503,19 @@
         <v>11</v>
       </c>
       <c r="T50" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E51" s="4">
         <v>8</v>
@@ -20530,16 +20527,16 @@
         <v>3</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I51" s="4">
         <v>7</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L51" s="4">
         <v>4</v>
@@ -20557,7 +20554,7 @@
         <v>1</v>
       </c>
       <c r="Q51" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R51" s="4">
         <v>9</v>
@@ -20571,16 +20568,16 @@
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E52" s="4">
         <v>8</v>
@@ -20592,16 +20589,16 @@
         <v>5</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I52" s="4" t="s">
         <v>5</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L52" s="4">
         <v>4</v>
@@ -20619,7 +20616,7 @@
         <v>1</v>
       </c>
       <c r="Q52" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R52" s="4">
         <v>9</v>
@@ -20633,16 +20630,16 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" s="4">
         <v>8</v>
@@ -20654,16 +20651,16 @@
         <v>5</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L53" s="4">
         <v>4</v>
@@ -20681,7 +20678,7 @@
         <v>1</v>
       </c>
       <c r="Q53" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R53" s="4">
         <v>9</v>
@@ -20695,7 +20692,7 @@
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B54" s="4">
         <v>12</v>
@@ -20704,7 +20701,7 @@
         <v>14</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" s="4">
         <v>8</v>
@@ -20716,16 +20713,16 @@
         <v>5</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L54" s="4">
         <v>4</v>
@@ -20743,7 +20740,7 @@
         <v>1</v>
       </c>
       <c r="Q54" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R54" s="4">
         <v>9</v>
@@ -20757,16 +20754,16 @@
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="4">
         <v>12</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E55" s="4">
         <v>8</v>
@@ -20778,22 +20775,22 @@
         <v>5</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>17</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L55" s="4">
         <v>4</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N55" s="4">
         <v>10</v>
@@ -20805,7 +20802,7 @@
         <v>1</v>
       </c>
       <c r="Q55" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R55" s="4">
         <v>9</v>
@@ -20819,16 +20816,16 @@
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B56" s="4">
         <v>12</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E56" s="4" t="s">
         <v>21</v>
@@ -20840,22 +20837,22 @@
         <v>5</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I56" s="4">
         <v>7</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L56" s="4">
         <v>4</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N56" s="4">
         <v>10</v>
@@ -20867,7 +20864,7 @@
         <v>1</v>
       </c>
       <c r="Q56" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R56" s="4">
         <v>9</v>
@@ -20881,16 +20878,16 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E57" s="4">
         <v>8</v>
@@ -20902,22 +20899,22 @@
         <v>5</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I57" s="4">
         <v>7</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L57" s="4">
         <v>4</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N57" s="4">
         <v>10</v>
@@ -20929,7 +20926,7 @@
         <v>1</v>
       </c>
       <c r="Q57" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R57" s="4">
         <v>9</v>
@@ -20943,16 +20940,16 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="4">
         <v>14</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E58" s="4">
         <v>8</v>
@@ -20964,22 +20961,22 @@
         <v>5</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I58" s="4">
         <v>7</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L58" s="4">
         <v>4</v>
       </c>
       <c r="M58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N58" s="4">
         <v>10</v>
@@ -20991,7 +20988,7 @@
         <v>1</v>
       </c>
       <c r="Q58" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R58" s="4">
         <v>9</v>
@@ -21005,7 +21002,7 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B59" s="4">
         <v>12</v>
@@ -21014,7 +21011,7 @@
         <v>14</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>21</v>
@@ -21026,22 +21023,22 @@
         <v>3</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I59" s="4">
         <v>7</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L59" s="4">
         <v>4</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N59" s="4">
         <v>10</v>
@@ -21053,7 +21050,7 @@
         <v>1</v>
       </c>
       <c r="Q59" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R59" s="4">
         <v>9</v>
@@ -21067,16 +21064,16 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C60" s="4">
         <v>14</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E60" s="4">
         <v>8</v>
@@ -21088,7 +21085,7 @@
         <v>3</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I60" s="4">
         <v>7</v>
@@ -21100,22 +21097,22 @@
         <v>3</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N60" s="4">
         <v>10</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P60" s="4">
         <v>1</v>
       </c>
       <c r="Q60" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R60" s="4">
         <v>9</v>
@@ -21129,16 +21126,16 @@
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C61" s="4">
         <v>14</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E61" s="4">
         <v>12</v>
@@ -21150,10 +21147,10 @@
         <v>5</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J61" s="4">
         <v>8</v>
@@ -21171,13 +21168,13 @@
         <v>10</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="P61" s="4">
         <v>1</v>
       </c>
       <c r="Q61" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R61" s="4">
         <v>9</v>
@@ -21194,13 +21191,13 @@
         <v>5</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E62" s="4">
         <v>8</v>
@@ -21209,19 +21206,19 @@
         <v>2</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I62" s="4">
         <v>7</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L62" s="4">
         <v>4</v>
@@ -21239,7 +21236,7 @@
         <v>1</v>
       </c>
       <c r="Q62" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R62" s="4">
         <v>9</v>
@@ -21253,16 +21250,16 @@
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E63" s="4">
         <v>8</v>
@@ -21274,22 +21271,22 @@
         <v>5</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I63" s="4">
         <v>7</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L63" s="4">
         <v>4</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N63" s="4">
         <v>10</v>
@@ -21301,7 +21298,7 @@
         <v>1</v>
       </c>
       <c r="Q63" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R63" s="4">
         <v>9</v>
@@ -21315,16 +21312,16 @@
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E64" s="4">
         <v>8</v>
@@ -21336,22 +21333,22 @@
         <v>5</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I64" s="4">
         <v>7</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L64" s="4">
         <v>4</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N64" s="4">
         <v>10</v>
@@ -21363,7 +21360,7 @@
         <v>1</v>
       </c>
       <c r="Q64" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R64" s="4">
         <v>9</v>
@@ -21377,13 +21374,13 @@
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D65" s="4">
         <v>2</v>
@@ -21392,28 +21389,28 @@
         <v>8</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G65" s="4">
         <v>5</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I65" s="4">
         <v>7</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L65" s="4">
         <v>4</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N65" s="4">
         <v>10</v>
@@ -21425,7 +21422,7 @@
         <v>1</v>
       </c>
       <c r="Q65" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R65" s="4">
         <v>9</v>
@@ -21439,7 +21436,7 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B66" s="4">
         <v>12</v>
@@ -21454,28 +21451,28 @@
         <v>21</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G66" s="4">
         <v>5</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I66" s="4">
         <v>7</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L66" s="4">
         <v>4</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N66" s="4">
         <v>10</v>
@@ -21487,7 +21484,7 @@
         <v>1</v>
       </c>
       <c r="Q66" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R66" s="4">
         <v>9</v>
@@ -21516,7 +21513,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>24</v>
@@ -21549,10 +21546,10 @@
         <v>66</v>
       </c>
       <c r="L1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>56</v>
@@ -26775,8 +26772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D9AD14E-5C41-B640-841F-A02FBCF76B8F}">
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -26810,7 +26807,7 @@
         <v>63</v>
       </c>
       <c r="J1" t="s">
-        <v>72</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
fixed more name issues
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F20A0F2-1266-4A4F-B33E-6952F17EE402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6F78F47F-2FBC-2C47-AD65-25B72E88A98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="1921-22" sheetId="19" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Lloyd</t>
   </si>
   <si>
-    <t>Phiipotts</t>
-  </si>
-  <si>
     <t>Richards</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>Thorpe</t>
+  </si>
+  <si>
+    <t>Philpotts</t>
   </si>
 </sst>
 </file>
@@ -896,97 +896,97 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>101</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>78</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>112</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>91</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -2398,7 +2398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B21AD3B-5CFD-9E48-9F5E-34B590DA3414}">
   <dimension ref="A1:X60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:X60"/>
     </sheetView>
   </sheetViews>
@@ -9191,8 +9191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA77E507-ADE4-EC47-A9C7-E6FD7EAE7A4E}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9226,22 +9226,22 @@
         <v>91</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
@@ -9457,37 +9457,37 @@
         <v>86</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>128</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>132</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>133</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>63</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N1" s="5" t="s">
         <v>34</v>
@@ -9502,22 +9502,22 @@
         <v>37</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="U1" s="5" t="s">
         <v>65</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -12063,7 +12063,7 @@
         <v>75</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>34</v>
@@ -12078,13 +12078,13 @@
         <v>37</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>39</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q1" s="7" t="s">
         <v>69</v>
@@ -12096,7 +12096,7 @@
         <v>65</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -13903,7 +13903,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H41" s="4">
         <v>3</v>
@@ -14812,25 +14812,25 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>62</v>
@@ -14851,7 +14851,7 @@
         <v>75</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>34</v>
@@ -14866,25 +14866,25 @@
         <v>37</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>39</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
added 96-97 and 98-99 seasons
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{6F78F47F-2FBC-2C47-AD65-25B72E88A98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9B1678-19E1-544C-AF8C-5115FCFB4EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="13" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="1921-22" sheetId="19" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="1993-94" sheetId="14" r:id="rId10"/>
     <sheet name="1994-95" sheetId="1" r:id="rId11"/>
     <sheet name="1995-96" sheetId="4" r:id="rId12"/>
+    <sheet name="1996-97" sheetId="23" r:id="rId13"/>
+    <sheet name="1998-99" sheetId="24" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="180">
   <si>
     <t>11+</t>
   </si>
@@ -498,6 +500,96 @@
   <si>
     <t>Philpotts</t>
   </si>
+  <si>
+    <t>Bonetti</t>
+  </si>
+  <si>
+    <t>Challinor</t>
+  </si>
+  <si>
+    <t>Jones L</t>
+  </si>
+  <si>
+    <t>Thorn</t>
+  </si>
+  <si>
+    <t>Woods</t>
+  </si>
+  <si>
+    <t>10#</t>
+  </si>
+  <si>
+    <t>6#</t>
+  </si>
+  <si>
+    <t>1+</t>
+  </si>
+  <si>
+    <t>5#</t>
+  </si>
+  <si>
+    <t>13*</t>
+  </si>
+  <si>
+    <t>Achterberg</t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Frail</t>
+  </si>
+  <si>
+    <t>Gibson</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Hinds</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Koumas</t>
+  </si>
+  <si>
+    <t>Mellon</t>
+  </si>
+  <si>
+    <t>Parkinson</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Sharps</t>
+  </si>
+  <si>
+    <t>Shepherd</t>
+  </si>
+  <si>
+    <t>Simonsen</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Thompson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>13+</t>
+  </si>
+  <si>
+    <t>2#</t>
+  </si>
 </sst>
 </file>
 
@@ -9187,11 +9279,4608 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D69175-2015-8C43-BCBA-332C8245AB32}">
+  <dimension ref="A1:Y52"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="W50" sqref="W50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>38</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>57</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4">
+        <v>9</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M2" s="4">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
+        <v>14</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>12</v>
+      </c>
+      <c r="S2" s="4">
+        <v>6</v>
+      </c>
+      <c r="T2" s="4">
+        <v>3</v>
+      </c>
+      <c r="U2" s="4">
+        <v>2</v>
+      </c>
+      <c r="V2" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4">
+        <v>9</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="M3" s="4">
+        <v>4</v>
+      </c>
+      <c r="P3" s="4">
+        <v>7</v>
+      </c>
+      <c r="S3" s="4">
+        <v>6</v>
+      </c>
+      <c r="T3" s="4">
+        <v>3</v>
+      </c>
+      <c r="U3" s="4">
+        <v>2</v>
+      </c>
+      <c r="V3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="4">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4">
+        <v>9</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="4">
+        <v>10</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N4" s="4">
+        <v>14</v>
+      </c>
+      <c r="P4" s="4">
+        <v>7</v>
+      </c>
+      <c r="S4" s="4">
+        <v>6</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U4" s="4">
+        <v>2</v>
+      </c>
+      <c r="V4" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4">
+        <v>9</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <v>4</v>
+      </c>
+      <c r="I5" s="4">
+        <v>10</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="4">
+        <v>12</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>13</v>
+      </c>
+      <c r="U5" s="4">
+        <v>2</v>
+      </c>
+      <c r="V5" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>9</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
+      <c r="L6" s="4">
+        <v>6</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>13</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="V6" s="4">
+        <v>5</v>
+      </c>
+      <c r="W6" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>8</v>
+      </c>
+      <c r="C7" s="4">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <v>4</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J7" s="4">
+        <v>7</v>
+      </c>
+      <c r="L7" s="4">
+        <v>12</v>
+      </c>
+      <c r="N7" s="4">
+        <v>13</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V7" s="4">
+        <v>5</v>
+      </c>
+      <c r="W7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4">
+        <v>9</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+      <c r="H8" s="4">
+        <v>4</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J8" s="4">
+        <v>13</v>
+      </c>
+      <c r="N8" s="4">
+        <v>12</v>
+      </c>
+      <c r="P8" s="4">
+        <v>7</v>
+      </c>
+      <c r="S8" s="4">
+        <v>6</v>
+      </c>
+      <c r="U8" s="4">
+        <v>2</v>
+      </c>
+      <c r="V8" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4">
+        <v>9</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4</v>
+      </c>
+      <c r="I9" s="4">
+        <v>10</v>
+      </c>
+      <c r="N9" s="4">
+        <v>12</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S9" s="4">
+        <v>6</v>
+      </c>
+      <c r="U9" s="4">
+        <v>2</v>
+      </c>
+      <c r="V9" s="4">
+        <v>5</v>
+      </c>
+      <c r="W9" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1</v>
+      </c>
+      <c r="H10" s="4">
+        <v>4</v>
+      </c>
+      <c r="I10" s="4">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4">
+        <v>13</v>
+      </c>
+      <c r="P10" s="4">
+        <v>7</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U10" s="4">
+        <v>2</v>
+      </c>
+      <c r="V10" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>4</v>
+      </c>
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
+      <c r="M11" s="4">
+        <v>12</v>
+      </c>
+      <c r="P11" s="4">
+        <v>7</v>
+      </c>
+      <c r="S11" s="4">
+        <v>6</v>
+      </c>
+      <c r="U11" s="4">
+        <v>2</v>
+      </c>
+      <c r="V11" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4">
+        <v>9</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>4</v>
+      </c>
+      <c r="L12" s="4">
+        <v>12</v>
+      </c>
+      <c r="P12" s="4">
+        <v>7</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" s="4">
+        <v>2</v>
+      </c>
+      <c r="V12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>8</v>
+      </c>
+      <c r="B13" s="4">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4">
+        <v>10</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="4">
+        <v>12</v>
+      </c>
+      <c r="J13" s="4">
+        <v>13</v>
+      </c>
+      <c r="L13" s="4">
+        <v>14</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="4">
+        <v>6</v>
+      </c>
+      <c r="U13" s="4">
+        <v>2</v>
+      </c>
+      <c r="V13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="4">
+        <v>11</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="I14" s="4">
+        <v>7</v>
+      </c>
+      <c r="J14" s="4">
+        <v>13</v>
+      </c>
+      <c r="P14" s="4">
+        <v>12</v>
+      </c>
+      <c r="S14" s="4">
+        <v>6</v>
+      </c>
+      <c r="U14" s="4">
+        <v>2</v>
+      </c>
+      <c r="V14" s="4">
+        <v>5</v>
+      </c>
+      <c r="X14" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>8</v>
+      </c>
+      <c r="B15" s="4">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="I15" s="4">
+        <v>7</v>
+      </c>
+      <c r="J15" s="4">
+        <v>13</v>
+      </c>
+      <c r="P15" s="4">
+        <v>12</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="U15" s="4">
+        <v>2</v>
+      </c>
+      <c r="V15" s="4">
+        <v>5</v>
+      </c>
+      <c r="X15" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <v>10</v>
+      </c>
+      <c r="D16" s="4">
+        <v>9</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="I16" s="4">
+        <v>7</v>
+      </c>
+      <c r="J16" s="4">
+        <v>13</v>
+      </c>
+      <c r="S16" s="4">
+        <v>6</v>
+      </c>
+      <c r="T16" s="4">
+        <v>3</v>
+      </c>
+      <c r="U16" s="4">
+        <v>2</v>
+      </c>
+      <c r="V16" s="4">
+        <v>5</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>8</v>
+      </c>
+      <c r="B17" s="4">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="4">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="4">
+        <v>13</v>
+      </c>
+      <c r="P17" s="4">
+        <v>12</v>
+      </c>
+      <c r="S17" s="4">
+        <v>6</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U17" s="4">
+        <v>2</v>
+      </c>
+      <c r="V17" s="4">
+        <v>5</v>
+      </c>
+      <c r="X17" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4">
+        <v>11</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="4">
+        <v>7</v>
+      </c>
+      <c r="J18" s="4">
+        <v>13</v>
+      </c>
+      <c r="L18" s="4">
+        <v>14</v>
+      </c>
+      <c r="P18" s="4">
+        <v>12</v>
+      </c>
+      <c r="S18" s="4">
+        <v>6</v>
+      </c>
+      <c r="U18" s="4">
+        <v>2</v>
+      </c>
+      <c r="V18" s="4">
+        <v>5</v>
+      </c>
+      <c r="X18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>8</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4">
+        <v>12</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1</v>
+      </c>
+      <c r="H19" s="4">
+        <v>4</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L19" s="4">
+        <v>14</v>
+      </c>
+      <c r="P19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>13</v>
+      </c>
+      <c r="S19" s="4">
+        <v>6</v>
+      </c>
+      <c r="U19" s="4">
+        <v>2</v>
+      </c>
+      <c r="V19" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4">
+        <v>7</v>
+      </c>
+      <c r="F20" s="4">
+        <v>10</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="4">
+        <v>11</v>
+      </c>
+      <c r="N20" s="4">
+        <v>8</v>
+      </c>
+      <c r="S20" s="4">
+        <v>6</v>
+      </c>
+      <c r="T20" s="4">
+        <v>3</v>
+      </c>
+      <c r="U20" s="4">
+        <v>2</v>
+      </c>
+      <c r="V20" s="4">
+        <v>5</v>
+      </c>
+      <c r="X20" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>12</v>
+      </c>
+      <c r="B21" s="4">
+        <v>14</v>
+      </c>
+      <c r="D21" s="4">
+        <v>7</v>
+      </c>
+      <c r="F21" s="4">
+        <v>10</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>8</v>
+      </c>
+      <c r="S21" s="4">
+        <v>6</v>
+      </c>
+      <c r="T21" s="4">
+        <v>3</v>
+      </c>
+      <c r="U21" s="4">
+        <v>2</v>
+      </c>
+      <c r="V21" s="4">
+        <v>5</v>
+      </c>
+      <c r="X21" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A22" s="4">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>14</v>
+      </c>
+      <c r="D22" s="4">
+        <v>7</v>
+      </c>
+      <c r="F22" s="4">
+        <v>10</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1</v>
+      </c>
+      <c r="H22" s="4">
+        <v>13</v>
+      </c>
+      <c r="J22" s="4">
+        <v>9</v>
+      </c>
+      <c r="L22" s="4">
+        <v>11</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T22" s="4">
+        <v>3</v>
+      </c>
+      <c r="U22" s="4">
+        <v>2</v>
+      </c>
+      <c r="V22" s="4">
+        <v>5</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A23" s="4">
+        <v>8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>12</v>
+      </c>
+      <c r="D23" s="4">
+        <v>7</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1</v>
+      </c>
+      <c r="H23" s="4">
+        <v>4</v>
+      </c>
+      <c r="I23" s="4">
+        <v>13</v>
+      </c>
+      <c r="J23" s="4">
+        <v>9</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="S23" s="4">
+        <v>6</v>
+      </c>
+      <c r="T23" s="4">
+        <v>3</v>
+      </c>
+      <c r="U23" s="4">
+        <v>2</v>
+      </c>
+      <c r="V23" s="4">
+        <v>5</v>
+      </c>
+      <c r="W23" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="4">
+        <v>11</v>
+      </c>
+      <c r="H24" s="4">
+        <v>4</v>
+      </c>
+      <c r="I24" s="4">
+        <v>12</v>
+      </c>
+      <c r="J24" s="4">
+        <v>14</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>13</v>
+      </c>
+      <c r="R24" s="4">
+        <v>1</v>
+      </c>
+      <c r="S24" s="4">
+        <v>6</v>
+      </c>
+      <c r="T24" s="4">
+        <v>3</v>
+      </c>
+      <c r="U24" s="4">
+        <v>2</v>
+      </c>
+      <c r="V24" s="4">
+        <v>5</v>
+      </c>
+      <c r="W24" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A25" s="4">
+        <v>8</v>
+      </c>
+      <c r="D25" s="4">
+        <v>7</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>4</v>
+      </c>
+      <c r="I25" s="4">
+        <v>12</v>
+      </c>
+      <c r="L25" s="4">
+        <v>14</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q25" s="4">
+        <v>13</v>
+      </c>
+      <c r="R25" s="4">
+        <v>1</v>
+      </c>
+      <c r="S25" s="4">
+        <v>6</v>
+      </c>
+      <c r="T25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U25" s="4">
+        <v>2</v>
+      </c>
+      <c r="V25" s="4">
+        <v>5</v>
+      </c>
+      <c r="W25" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>8</v>
+      </c>
+      <c r="D26" s="4">
+        <v>7</v>
+      </c>
+      <c r="F26" s="4">
+        <v>14</v>
+      </c>
+      <c r="H26" s="4">
+        <v>4</v>
+      </c>
+      <c r="I26" s="4">
+        <v>12</v>
+      </c>
+      <c r="J26" s="4">
+        <v>13</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="R26" s="4">
+        <v>1</v>
+      </c>
+      <c r="S26" s="4">
+        <v>6</v>
+      </c>
+      <c r="T26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U26" s="4">
+        <v>2</v>
+      </c>
+      <c r="V26" s="4">
+        <v>5</v>
+      </c>
+      <c r="W26" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A27" s="4">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4">
+        <v>7</v>
+      </c>
+      <c r="F27" s="4">
+        <v>11</v>
+      </c>
+      <c r="H27" s="4">
+        <v>4</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="4">
+        <v>13</v>
+      </c>
+      <c r="P27" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q27" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="R27" s="4">
+        <v>1</v>
+      </c>
+      <c r="S27" s="4">
+        <v>6</v>
+      </c>
+      <c r="U27" s="4">
+        <v>2</v>
+      </c>
+      <c r="V27" s="4">
+        <v>5</v>
+      </c>
+      <c r="W27" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A28" s="4">
+        <v>8</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="4">
+        <v>9</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J28" s="4">
+        <v>12</v>
+      </c>
+      <c r="L28" s="4">
+        <v>14</v>
+      </c>
+      <c r="M28" s="4">
+        <v>4</v>
+      </c>
+      <c r="P28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q28" s="4">
+        <v>13</v>
+      </c>
+      <c r="R28" s="4">
+        <v>1</v>
+      </c>
+      <c r="S28" s="4">
+        <v>6</v>
+      </c>
+      <c r="U28" s="4">
+        <v>2</v>
+      </c>
+      <c r="V28" s="4">
+        <v>5</v>
+      </c>
+      <c r="W28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A29" s="4">
+        <v>13</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1</v>
+      </c>
+      <c r="I29" s="4">
+        <v>14</v>
+      </c>
+      <c r="L29" s="4">
+        <v>11</v>
+      </c>
+      <c r="M29" s="4">
+        <v>4</v>
+      </c>
+      <c r="N29" s="4">
+        <v>10</v>
+      </c>
+      <c r="P29" s="4">
+        <v>12</v>
+      </c>
+      <c r="S29" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T29" s="4">
+        <v>3</v>
+      </c>
+      <c r="U29" s="4">
+        <v>2</v>
+      </c>
+      <c r="V29" s="4">
+        <v>5</v>
+      </c>
+      <c r="W29" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A30" s="4">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4">
+        <v>12</v>
+      </c>
+      <c r="D30" s="4">
+        <v>7</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1</v>
+      </c>
+      <c r="I30" s="4">
+        <v>9</v>
+      </c>
+      <c r="L30" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" s="4">
+        <v>4</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q30" s="4">
+        <v>13</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T30" s="4">
+        <v>3</v>
+      </c>
+      <c r="U30" s="4">
+        <v>2</v>
+      </c>
+      <c r="V30" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="4">
+        <v>12</v>
+      </c>
+      <c r="D31" s="4">
+        <v>7</v>
+      </c>
+      <c r="F31" s="4">
+        <v>9</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H31" s="4">
+        <v>5</v>
+      </c>
+      <c r="L31" s="4">
+        <v>14</v>
+      </c>
+      <c r="M31" s="4">
+        <v>4</v>
+      </c>
+      <c r="N31" s="4">
+        <v>13</v>
+      </c>
+      <c r="P31" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>11</v>
+      </c>
+      <c r="S31" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U31" s="4">
+        <v>2</v>
+      </c>
+      <c r="W31" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="4">
+        <v>12</v>
+      </c>
+      <c r="D32" s="4">
+        <v>7</v>
+      </c>
+      <c r="F32" s="4">
+        <v>9</v>
+      </c>
+      <c r="H32" s="4">
+        <v>5</v>
+      </c>
+      <c r="I32" s="4">
+        <v>14</v>
+      </c>
+      <c r="M32" s="4">
+        <v>4</v>
+      </c>
+      <c r="N32" s="4">
+        <v>13</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>11</v>
+      </c>
+      <c r="R32" s="4">
+        <v>1</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="U32" s="4">
+        <v>2</v>
+      </c>
+      <c r="W32" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33" s="4">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4">
+        <v>12</v>
+      </c>
+      <c r="D33" s="4">
+        <v>7</v>
+      </c>
+      <c r="F33" s="4">
+        <v>9</v>
+      </c>
+      <c r="H33" s="4">
+        <v>5</v>
+      </c>
+      <c r="I33" s="4">
+        <v>14</v>
+      </c>
+      <c r="M33" s="4">
+        <v>4</v>
+      </c>
+      <c r="N33" s="4">
+        <v>13</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>11</v>
+      </c>
+      <c r="R33" s="4">
+        <v>1</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="U33" s="4">
+        <v>2</v>
+      </c>
+      <c r="W33" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34" s="4">
+        <v>8</v>
+      </c>
+      <c r="D34" s="4">
+        <v>7</v>
+      </c>
+      <c r="F34" s="4">
+        <v>9</v>
+      </c>
+      <c r="H34" s="4">
+        <v>5</v>
+      </c>
+      <c r="I34" s="4">
+        <v>14</v>
+      </c>
+      <c r="M34" s="4">
+        <v>4</v>
+      </c>
+      <c r="N34" s="4">
+        <v>13</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R34" s="4">
+        <v>1</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T34" s="4">
+        <v>12</v>
+      </c>
+      <c r="U34" s="4">
+        <v>2</v>
+      </c>
+      <c r="W34" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="B35" s="4">
+        <v>14</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="4">
+        <v>9</v>
+      </c>
+      <c r="I35" s="4">
+        <v>6</v>
+      </c>
+      <c r="J35" s="4">
+        <v>13</v>
+      </c>
+      <c r="M35" s="4">
+        <v>4</v>
+      </c>
+      <c r="N35" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R35" s="4">
+        <v>1</v>
+      </c>
+      <c r="T35" s="4">
+        <v>12</v>
+      </c>
+      <c r="U35" s="4">
+        <v>2</v>
+      </c>
+      <c r="W35" s="4">
+        <v>3</v>
+      </c>
+      <c r="X35" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C36" s="4">
+        <v>10</v>
+      </c>
+      <c r="F36" s="4">
+        <v>9</v>
+      </c>
+      <c r="I36" s="4">
+        <v>6</v>
+      </c>
+      <c r="J36" s="4">
+        <v>13</v>
+      </c>
+      <c r="L36" s="4">
+        <v>7</v>
+      </c>
+      <c r="M36" s="4">
+        <v>4</v>
+      </c>
+      <c r="N36" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R36" s="4">
+        <v>1</v>
+      </c>
+      <c r="T36" s="4">
+        <v>12</v>
+      </c>
+      <c r="U36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="W36" s="4">
+        <v>3</v>
+      </c>
+      <c r="X36" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="C37" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D37" s="4">
+        <v>12</v>
+      </c>
+      <c r="F37" s="4">
+        <v>9</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="4">
+        <v>13</v>
+      </c>
+      <c r="L37" s="4">
+        <v>7</v>
+      </c>
+      <c r="M37" s="4">
+        <v>4</v>
+      </c>
+      <c r="N37" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q37" s="4">
+        <v>14</v>
+      </c>
+      <c r="R37" s="4">
+        <v>1</v>
+      </c>
+      <c r="T37" s="4">
+        <v>11</v>
+      </c>
+      <c r="U37" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="W37" s="4">
+        <v>3</v>
+      </c>
+      <c r="X37" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A38" s="4">
+        <v>12</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="4">
+        <v>7</v>
+      </c>
+      <c r="H38" s="4">
+        <v>5</v>
+      </c>
+      <c r="I38" s="4">
+        <v>10</v>
+      </c>
+      <c r="J38" s="4">
+        <v>13</v>
+      </c>
+      <c r="L38" s="4">
+        <v>14</v>
+      </c>
+      <c r="M38" s="4">
+        <v>4</v>
+      </c>
+      <c r="N38" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R38" s="4">
+        <v>1</v>
+      </c>
+      <c r="S38" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T38" s="4">
+        <v>3</v>
+      </c>
+      <c r="W38" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A39" s="4">
+        <v>12</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="4">
+        <v>7</v>
+      </c>
+      <c r="E39" s="4">
+        <v>4</v>
+      </c>
+      <c r="H39" s="4">
+        <v>5</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L39" s="4">
+        <v>14</v>
+      </c>
+      <c r="N39" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>11</v>
+      </c>
+      <c r="R39" s="4">
+        <v>1</v>
+      </c>
+      <c r="S39" s="4">
+        <v>6</v>
+      </c>
+      <c r="T39" s="4">
+        <v>3</v>
+      </c>
+      <c r="W39" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C40" s="4">
+        <v>12</v>
+      </c>
+      <c r="D40" s="4">
+        <v>7</v>
+      </c>
+      <c r="H40" s="4">
+        <v>4</v>
+      </c>
+      <c r="I40" s="4">
+        <v>10</v>
+      </c>
+      <c r="J40" s="4">
+        <v>13</v>
+      </c>
+      <c r="N40" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R40" s="4">
+        <v>1</v>
+      </c>
+      <c r="S40" s="4">
+        <v>6</v>
+      </c>
+      <c r="T40" s="4">
+        <v>3</v>
+      </c>
+      <c r="W40" s="4">
+        <v>2</v>
+      </c>
+      <c r="X40" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="4">
+        <v>12</v>
+      </c>
+      <c r="D41" s="4">
+        <v>7</v>
+      </c>
+      <c r="F41" s="4">
+        <v>14</v>
+      </c>
+      <c r="H41" s="4">
+        <v>11</v>
+      </c>
+      <c r="I41" s="4">
+        <v>10</v>
+      </c>
+      <c r="J41" s="4">
+        <v>13</v>
+      </c>
+      <c r="M41" s="4">
+        <v>4</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R41" s="4">
+        <v>1</v>
+      </c>
+      <c r="S41" s="4">
+        <v>6</v>
+      </c>
+      <c r="T41" s="4">
+        <v>3</v>
+      </c>
+      <c r="W41" s="4">
+        <v>2</v>
+      </c>
+      <c r="X41" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A42" s="4">
+        <v>8</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F42" s="4">
+        <v>9</v>
+      </c>
+      <c r="H42" s="4">
+        <v>5</v>
+      </c>
+      <c r="I42" s="4">
+        <v>10</v>
+      </c>
+      <c r="L42" s="4">
+        <v>11</v>
+      </c>
+      <c r="M42" s="4">
+        <v>4</v>
+      </c>
+      <c r="P42" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q42" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="R42" s="4">
+        <v>1</v>
+      </c>
+      <c r="S42" s="4">
+        <v>6</v>
+      </c>
+      <c r="T42" s="4">
+        <v>3</v>
+      </c>
+      <c r="W42" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A43" s="4">
+        <v>12</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E43" s="4">
+        <v>14</v>
+      </c>
+      <c r="F43" s="4">
+        <v>9</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I43" s="4">
+        <v>10</v>
+      </c>
+      <c r="J43" s="4">
+        <v>8</v>
+      </c>
+      <c r="L43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M43" s="4">
+        <v>4</v>
+      </c>
+      <c r="P43" s="4">
+        <v>13</v>
+      </c>
+      <c r="R43" s="4">
+        <v>1</v>
+      </c>
+      <c r="S43" s="4">
+        <v>6</v>
+      </c>
+      <c r="T43" s="4">
+        <v>3</v>
+      </c>
+      <c r="W43" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A44" s="4">
+        <v>8</v>
+      </c>
+      <c r="C44" s="4">
+        <v>12</v>
+      </c>
+      <c r="E44" s="4">
+        <v>5</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I44" s="4">
+        <v>10</v>
+      </c>
+      <c r="J44" s="4">
+        <v>9</v>
+      </c>
+      <c r="L44" s="4">
+        <v>13</v>
+      </c>
+      <c r="M44" s="4">
+        <v>4</v>
+      </c>
+      <c r="P44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R44" s="4">
+        <v>1</v>
+      </c>
+      <c r="S44" s="4">
+        <v>6</v>
+      </c>
+      <c r="T44" s="4">
+        <v>3</v>
+      </c>
+      <c r="W44" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="4">
+        <v>12</v>
+      </c>
+      <c r="E45" s="4">
+        <v>5</v>
+      </c>
+      <c r="F45" s="4">
+        <v>13</v>
+      </c>
+      <c r="I45" s="4">
+        <v>10</v>
+      </c>
+      <c r="J45" s="4">
+        <v>9</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M45" s="4">
+        <v>4</v>
+      </c>
+      <c r="P45" s="4">
+        <v>7</v>
+      </c>
+      <c r="R45" s="4">
+        <v>1</v>
+      </c>
+      <c r="S45" s="4">
+        <v>6</v>
+      </c>
+      <c r="T45" s="4">
+        <v>3</v>
+      </c>
+      <c r="W45" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A46" s="4">
+        <v>14</v>
+      </c>
+      <c r="C46" s="4">
+        <v>12</v>
+      </c>
+      <c r="E46" s="4">
+        <v>5</v>
+      </c>
+      <c r="F46" s="4">
+        <v>8</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J46" s="4">
+        <v>9</v>
+      </c>
+      <c r="K46" s="4">
+        <v>11</v>
+      </c>
+      <c r="M46" s="4">
+        <v>4</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R46" s="4">
+        <v>1</v>
+      </c>
+      <c r="S46" s="4">
+        <v>6</v>
+      </c>
+      <c r="W46" s="4">
+        <v>2</v>
+      </c>
+      <c r="Y46" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="4">
+        <v>12</v>
+      </c>
+      <c r="F47" s="4">
+        <v>13</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J47" s="4">
+        <v>9</v>
+      </c>
+      <c r="K47" s="4">
+        <v>11</v>
+      </c>
+      <c r="L47" s="4">
+        <v>14</v>
+      </c>
+      <c r="M47" s="4">
+        <v>4</v>
+      </c>
+      <c r="P47" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R47" s="4">
+        <v>1</v>
+      </c>
+      <c r="S47" s="4">
+        <v>6</v>
+      </c>
+      <c r="T47" s="4">
+        <v>3</v>
+      </c>
+      <c r="W47" s="4">
+        <v>2</v>
+      </c>
+      <c r="X47" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A48" s="4">
+        <v>12</v>
+      </c>
+      <c r="C48" s="4">
+        <v>14</v>
+      </c>
+      <c r="F48" s="4">
+        <v>8</v>
+      </c>
+      <c r="I48" s="4">
+        <v>10</v>
+      </c>
+      <c r="J48" s="4">
+        <v>9</v>
+      </c>
+      <c r="K48" s="4">
+        <v>11</v>
+      </c>
+      <c r="L48" s="4">
+        <v>13</v>
+      </c>
+      <c r="M48" s="4">
+        <v>4</v>
+      </c>
+      <c r="P48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="R48" s="4">
+        <v>1</v>
+      </c>
+      <c r="S48" s="4">
+        <v>6</v>
+      </c>
+      <c r="T48" s="4">
+        <v>3</v>
+      </c>
+      <c r="W48" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="X48" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A49" s="4">
+        <v>12</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8</v>
+      </c>
+      <c r="I49" s="4">
+        <v>10</v>
+      </c>
+      <c r="J49" s="4">
+        <v>9</v>
+      </c>
+      <c r="K49" s="4">
+        <v>11</v>
+      </c>
+      <c r="M49" s="4">
+        <v>4</v>
+      </c>
+      <c r="P49" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R49" s="4">
+        <v>1</v>
+      </c>
+      <c r="S49" s="4">
+        <v>6</v>
+      </c>
+      <c r="T49" s="4">
+        <v>3</v>
+      </c>
+      <c r="W49" s="4">
+        <v>2</v>
+      </c>
+      <c r="X49" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A50" s="4">
+        <v>12</v>
+      </c>
+      <c r="C50" s="4">
+        <v>14</v>
+      </c>
+      <c r="F50" s="4">
+        <v>8</v>
+      </c>
+      <c r="I50" s="4">
+        <v>10</v>
+      </c>
+      <c r="J50" s="4">
+        <v>9</v>
+      </c>
+      <c r="K50" s="4">
+        <v>11</v>
+      </c>
+      <c r="M50" s="4">
+        <v>4</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="R50" s="4">
+        <v>1</v>
+      </c>
+      <c r="S50" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="T50" s="4">
+        <v>3</v>
+      </c>
+      <c r="W50" s="4">
+        <v>2</v>
+      </c>
+      <c r="X50" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A51" s="4">
+        <v>8</v>
+      </c>
+      <c r="I51" s="4">
+        <v>10</v>
+      </c>
+      <c r="J51" s="4">
+        <v>9</v>
+      </c>
+      <c r="K51" s="4">
+        <v>11</v>
+      </c>
+      <c r="M51" s="4">
+        <v>4</v>
+      </c>
+      <c r="P51" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q51" s="4">
+        <v>13</v>
+      </c>
+      <c r="R51" s="4">
+        <v>1</v>
+      </c>
+      <c r="S51" s="4">
+        <v>6</v>
+      </c>
+      <c r="T51" s="4">
+        <v>3</v>
+      </c>
+      <c r="W51" s="4">
+        <v>2</v>
+      </c>
+      <c r="X51" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A52" s="4">
+        <v>8</v>
+      </c>
+      <c r="C52" s="4">
+        <v>7</v>
+      </c>
+      <c r="I52" s="4">
+        <v>10</v>
+      </c>
+      <c r="K52" s="4">
+        <v>11</v>
+      </c>
+      <c r="L52" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M52" s="4">
+        <v>4</v>
+      </c>
+      <c r="P52" s="4">
+        <v>12</v>
+      </c>
+      <c r="R52" s="4">
+        <v>1</v>
+      </c>
+      <c r="S52" s="4">
+        <v>6</v>
+      </c>
+      <c r="T52" s="4">
+        <v>3</v>
+      </c>
+      <c r="W52" s="4">
+        <v>2</v>
+      </c>
+      <c r="X52" s="4">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93365371-A62D-3C43-8BC3-6C95C3C5319E}">
+  <dimension ref="A1:AB53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S35" sqref="S35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" t="s">
+        <v>40</v>
+      </c>
+      <c r="T1" t="s">
+        <v>169</v>
+      </c>
+      <c r="U1" t="s">
+        <v>170</v>
+      </c>
+      <c r="V1" t="s">
+        <v>171</v>
+      </c>
+      <c r="W1" t="s">
+        <v>172</v>
+      </c>
+      <c r="X1" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>174</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4">
+        <v>9</v>
+      </c>
+      <c r="N2" s="4"/>
+      <c r="O2">
+        <v>4</v>
+      </c>
+      <c r="P2">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2">
+        <v>12</v>
+      </c>
+      <c r="U2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2">
+        <v>8</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4">
+        <v>9</v>
+      </c>
+      <c r="N3" s="4"/>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <v>11</v>
+      </c>
+      <c r="R3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3">
+        <v>10</v>
+      </c>
+      <c r="V3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4">
+        <v>4</v>
+      </c>
+      <c r="P4">
+        <v>11</v>
+      </c>
+      <c r="R4">
+        <v>7</v>
+      </c>
+      <c r="T4">
+        <v>10</v>
+      </c>
+      <c r="U4" t="s">
+        <v>14</v>
+      </c>
+      <c r="V4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="AA4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5" s="4">
+        <v>11</v>
+      </c>
+      <c r="L5" s="4"/>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>8</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>12</v>
+      </c>
+      <c r="T5" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="4">
+        <v>11</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6">
+        <v>14</v>
+      </c>
+      <c r="N6" s="4"/>
+      <c r="O6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>12</v>
+      </c>
+      <c r="T6">
+        <v>7</v>
+      </c>
+      <c r="U6" t="s">
+        <v>14</v>
+      </c>
+      <c r="W6" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="4"/>
+      <c r="M7">
+        <v>13</v>
+      </c>
+      <c r="N7" s="4"/>
+      <c r="P7">
+        <v>12</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" t="s">
+        <v>49</v>
+      </c>
+      <c r="S7">
+        <v>8</v>
+      </c>
+      <c r="T7">
+        <v>10</v>
+      </c>
+      <c r="U7">
+        <v>14</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="P8">
+        <v>7</v>
+      </c>
+      <c r="R8">
+        <v>12</v>
+      </c>
+      <c r="S8">
+        <v>4</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="V8">
+        <v>8</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="K9" s="4">
+        <v>11</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9">
+        <v>12</v>
+      </c>
+      <c r="N9" s="4">
+        <v>14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9">
+        <v>13</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <v>9</v>
+      </c>
+      <c r="V9" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4">
+        <v>12</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N10" s="4">
+        <v>15</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10" t="s">
+        <v>46</v>
+      </c>
+      <c r="R10">
+        <v>14</v>
+      </c>
+      <c r="S10">
+        <v>4</v>
+      </c>
+      <c r="T10">
+        <v>10</v>
+      </c>
+      <c r="V10">
+        <v>8</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="AA10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11">
+        <v>13</v>
+      </c>
+      <c r="K11" s="4">
+        <v>12</v>
+      </c>
+      <c r="L11" s="4"/>
+      <c r="M11" t="s">
+        <v>5</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>14</v>
+      </c>
+      <c r="S11">
+        <v>10</v>
+      </c>
+      <c r="T11">
+        <v>9</v>
+      </c>
+      <c r="V11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12">
+        <v>15</v>
+      </c>
+      <c r="K12" s="4">
+        <v>12</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12">
+        <v>7</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="S12">
+        <v>10</v>
+      </c>
+      <c r="T12">
+        <v>9</v>
+      </c>
+      <c r="V12" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="4"/>
+      <c r="M13">
+        <v>7</v>
+      </c>
+      <c r="N13" s="4">
+        <v>12</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="R13">
+        <v>14</v>
+      </c>
+      <c r="S13" t="s">
+        <v>155</v>
+      </c>
+      <c r="T13" t="s">
+        <v>11</v>
+      </c>
+      <c r="V13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>13</v>
+      </c>
+      <c r="K14" s="4">
+        <v>11</v>
+      </c>
+      <c r="L14" s="4"/>
+      <c r="M14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="4">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="R14">
+        <v>12</v>
+      </c>
+      <c r="V14" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15" s="4">
+        <v>14</v>
+      </c>
+      <c r="L15" s="4"/>
+      <c r="M15" t="s">
+        <v>5</v>
+      </c>
+      <c r="N15" s="4">
+        <v>11</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>10</v>
+      </c>
+      <c r="R15">
+        <v>12</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16" s="4">
+        <v>12</v>
+      </c>
+      <c r="L16" s="4"/>
+      <c r="M16">
+        <v>7</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="P16">
+        <v>10</v>
+      </c>
+      <c r="V16">
+        <v>8</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>9</v>
+      </c>
+      <c r="K17" s="4">
+        <v>12</v>
+      </c>
+      <c r="L17" s="4"/>
+      <c r="M17" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="4">
+        <v>13</v>
+      </c>
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>10</v>
+      </c>
+      <c r="R17">
+        <v>14</v>
+      </c>
+      <c r="V17">
+        <v>8</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="I18">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="4">
+        <v>12</v>
+      </c>
+      <c r="L18" s="4">
+        <v>13</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>10</v>
+      </c>
+      <c r="R18">
+        <v>14</v>
+      </c>
+      <c r="V18">
+        <v>8</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>5</v>
+      </c>
+      <c r="I19">
+        <v>6</v>
+      </c>
+      <c r="J19" t="s">
+        <v>11</v>
+      </c>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4">
+        <v>12</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>10</v>
+      </c>
+      <c r="R19">
+        <v>14</v>
+      </c>
+      <c r="V19">
+        <v>8</v>
+      </c>
+      <c r="Z19">
+        <v>11</v>
+      </c>
+      <c r="AA19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>9</v>
+      </c>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4">
+        <v>11</v>
+      </c>
+      <c r="M20" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20" t="s">
+        <v>16</v>
+      </c>
+      <c r="S20">
+        <v>12</v>
+      </c>
+      <c r="T20">
+        <v>16</v>
+      </c>
+      <c r="V20">
+        <v>8</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>158</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>9</v>
+      </c>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4">
+        <v>12</v>
+      </c>
+      <c r="N21" s="4">
+        <v>7</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21" t="s">
+        <v>16</v>
+      </c>
+      <c r="R21">
+        <v>14</v>
+      </c>
+      <c r="V21">
+        <v>8</v>
+      </c>
+      <c r="Z21">
+        <v>11</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="G22" t="s">
+        <v>158</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>9</v>
+      </c>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4">
+        <v>12</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O22">
+        <v>4</v>
+      </c>
+      <c r="P22">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>14</v>
+      </c>
+      <c r="V22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z22">
+        <v>11</v>
+      </c>
+      <c r="AA22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>9</v>
+      </c>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4">
+        <v>12</v>
+      </c>
+      <c r="N23" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="P23">
+        <v>10</v>
+      </c>
+      <c r="R23">
+        <v>14</v>
+      </c>
+      <c r="V23">
+        <v>8</v>
+      </c>
+      <c r="Z23">
+        <v>11</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>14</v>
+      </c>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4">
+        <v>12</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="P24">
+        <v>10</v>
+      </c>
+      <c r="R24">
+        <v>14</v>
+      </c>
+      <c r="V24">
+        <v>8</v>
+      </c>
+      <c r="Z24">
+        <v>11</v>
+      </c>
+      <c r="AA24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>13</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4">
+        <v>9</v>
+      </c>
+      <c r="N25" s="4">
+        <v>4</v>
+      </c>
+      <c r="P25" t="s">
+        <v>9</v>
+      </c>
+      <c r="R25" t="s">
+        <v>49</v>
+      </c>
+      <c r="T25">
+        <v>14</v>
+      </c>
+      <c r="V25">
+        <v>8</v>
+      </c>
+      <c r="Z25">
+        <v>11</v>
+      </c>
+      <c r="AA25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4">
+        <v>9</v>
+      </c>
+      <c r="M26">
+        <v>13</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="P26">
+        <v>10</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>21</v>
+      </c>
+      <c r="R26">
+        <v>12</v>
+      </c>
+      <c r="T26">
+        <v>14</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4">
+        <v>9</v>
+      </c>
+      <c r="M27">
+        <v>7</v>
+      </c>
+      <c r="N27" s="4">
+        <v>13</v>
+      </c>
+      <c r="P27" t="s">
+        <v>155</v>
+      </c>
+      <c r="T27">
+        <v>11</v>
+      </c>
+      <c r="V27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z27">
+        <v>14</v>
+      </c>
+      <c r="AA27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4">
+        <v>9</v>
+      </c>
+      <c r="M28" t="s">
+        <v>49</v>
+      </c>
+      <c r="N28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28">
+        <v>13</v>
+      </c>
+      <c r="R28">
+        <v>12</v>
+      </c>
+      <c r="T28" t="s">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>8</v>
+      </c>
+      <c r="Z28">
+        <v>14</v>
+      </c>
+      <c r="AA28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>179</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M29" t="s">
+        <v>17</v>
+      </c>
+      <c r="N29" s="4">
+        <v>10</v>
+      </c>
+      <c r="O29">
+        <v>4</v>
+      </c>
+      <c r="P29">
+        <v>13</v>
+      </c>
+      <c r="R29">
+        <v>12</v>
+      </c>
+      <c r="T29">
+        <v>14</v>
+      </c>
+      <c r="V29">
+        <v>8</v>
+      </c>
+      <c r="Z29">
+        <v>11</v>
+      </c>
+      <c r="AA29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>14</v>
+      </c>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N30" s="4">
+        <v>10</v>
+      </c>
+      <c r="O30">
+        <v>4</v>
+      </c>
+      <c r="P30">
+        <v>7</v>
+      </c>
+      <c r="V30">
+        <v>8</v>
+      </c>
+      <c r="Z30">
+        <v>11</v>
+      </c>
+      <c r="AA30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31" t="s">
+        <v>47</v>
+      </c>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="N31" s="4">
+        <v>7</v>
+      </c>
+      <c r="O31">
+        <v>4</v>
+      </c>
+      <c r="P31">
+        <v>10</v>
+      </c>
+      <c r="T31">
+        <v>13</v>
+      </c>
+      <c r="V31">
+        <v>8</v>
+      </c>
+      <c r="Z31">
+        <v>11</v>
+      </c>
+      <c r="AA31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>5</v>
+      </c>
+      <c r="I32" t="s">
+        <v>13</v>
+      </c>
+      <c r="J32">
+        <v>9</v>
+      </c>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="N32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O32">
+        <v>4</v>
+      </c>
+      <c r="P32">
+        <v>10</v>
+      </c>
+      <c r="Q32">
+        <v>14</v>
+      </c>
+      <c r="R32">
+        <v>12</v>
+      </c>
+      <c r="T32">
+        <v>13</v>
+      </c>
+      <c r="V32">
+        <v>8</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>2</v>
+      </c>
+      <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>9</v>
+      </c>
+      <c r="K33" s="4">
+        <v>16</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="N33" s="4">
+        <v>7</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33" t="s">
+        <v>155</v>
+      </c>
+      <c r="R33">
+        <v>12</v>
+      </c>
+      <c r="T33">
+        <v>14</v>
+      </c>
+      <c r="V33">
+        <v>8</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="K34" s="4">
+        <v>14</v>
+      </c>
+      <c r="L34" s="4"/>
+      <c r="M34">
+        <v>13</v>
+      </c>
+      <c r="N34" s="4">
+        <v>7</v>
+      </c>
+      <c r="O34">
+        <v>4</v>
+      </c>
+      <c r="R34">
+        <v>12</v>
+      </c>
+      <c r="S34" t="s">
+        <v>46</v>
+      </c>
+      <c r="T34" t="s">
+        <v>11</v>
+      </c>
+      <c r="V34">
+        <v>8</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>5</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>11</v>
+      </c>
+      <c r="I35">
+        <v>6</v>
+      </c>
+      <c r="J35">
+        <v>14</v>
+      </c>
+      <c r="K35" s="4">
+        <v>13</v>
+      </c>
+      <c r="L35" s="4"/>
+      <c r="N35" s="4">
+        <v>7</v>
+      </c>
+      <c r="O35">
+        <v>4</v>
+      </c>
+      <c r="S35" t="s">
+        <v>8</v>
+      </c>
+      <c r="T35" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z35">
+        <v>10</v>
+      </c>
+      <c r="AA35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>12</v>
+      </c>
+      <c r="K36" s="4">
+        <v>11</v>
+      </c>
+      <c r="L36" s="4"/>
+      <c r="M36">
+        <v>14</v>
+      </c>
+      <c r="N36" s="4">
+        <v>7</v>
+      </c>
+      <c r="O36">
+        <v>4</v>
+      </c>
+      <c r="S36" t="s">
+        <v>11</v>
+      </c>
+      <c r="T36" t="s">
+        <v>10</v>
+      </c>
+      <c r="V36">
+        <v>8</v>
+      </c>
+      <c r="Z36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>2</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>9</v>
+      </c>
+      <c r="I37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37">
+        <v>14</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L37" s="4"/>
+      <c r="N37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O37">
+        <v>4</v>
+      </c>
+      <c r="S37">
+        <v>12</v>
+      </c>
+      <c r="T37">
+        <v>13</v>
+      </c>
+      <c r="V37">
+        <v>8</v>
+      </c>
+      <c r="Z37">
+        <v>10</v>
+      </c>
+      <c r="AA37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <v>5</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="4">
+        <v>11</v>
+      </c>
+      <c r="L38" s="4"/>
+      <c r="M38">
+        <v>13</v>
+      </c>
+      <c r="N38" s="4">
+        <v>7</v>
+      </c>
+      <c r="O38">
+        <v>4</v>
+      </c>
+      <c r="S38">
+        <v>12</v>
+      </c>
+      <c r="T38" t="s">
+        <v>47</v>
+      </c>
+      <c r="V38">
+        <v>8</v>
+      </c>
+      <c r="Z38">
+        <v>10</v>
+      </c>
+      <c r="AA38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>2</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>6</v>
+      </c>
+      <c r="K39" s="4">
+        <v>11</v>
+      </c>
+      <c r="L39" s="4"/>
+      <c r="M39">
+        <v>13</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="O39">
+        <v>4</v>
+      </c>
+      <c r="S39">
+        <v>9</v>
+      </c>
+      <c r="V39">
+        <v>8</v>
+      </c>
+      <c r="Z39">
+        <v>10</v>
+      </c>
+      <c r="AA39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="J40">
+        <v>14</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" s="4">
+        <v>12</v>
+      </c>
+      <c r="M40">
+        <v>13</v>
+      </c>
+      <c r="N40" s="4">
+        <v>7</v>
+      </c>
+      <c r="O40">
+        <v>4</v>
+      </c>
+      <c r="S40" t="s">
+        <v>11</v>
+      </c>
+      <c r="T40">
+        <v>8</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>14</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="4">
+        <v>12</v>
+      </c>
+      <c r="M41">
+        <v>13</v>
+      </c>
+      <c r="N41" s="4">
+        <v>7</v>
+      </c>
+      <c r="O41">
+        <v>4</v>
+      </c>
+      <c r="S41" t="s">
+        <v>47</v>
+      </c>
+      <c r="T41">
+        <v>8</v>
+      </c>
+      <c r="Z41">
+        <v>10</v>
+      </c>
+      <c r="AA41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>14</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L42" s="4">
+        <v>12</v>
+      </c>
+      <c r="M42">
+        <v>13</v>
+      </c>
+      <c r="N42" s="4">
+        <v>7</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="S42" t="s">
+        <v>47</v>
+      </c>
+      <c r="T42">
+        <v>8</v>
+      </c>
+      <c r="Z42">
+        <v>10</v>
+      </c>
+      <c r="AA42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43">
+        <v>14</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>6</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L43" s="4">
+        <v>12</v>
+      </c>
+      <c r="M43">
+        <v>13</v>
+      </c>
+      <c r="N43" s="4">
+        <v>7</v>
+      </c>
+      <c r="O43">
+        <v>4</v>
+      </c>
+      <c r="S43" t="s">
+        <v>11</v>
+      </c>
+      <c r="T43">
+        <v>8</v>
+      </c>
+      <c r="Z43">
+        <v>10</v>
+      </c>
+      <c r="AA43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="K44" s="4">
+        <v>14</v>
+      </c>
+      <c r="L44" s="4">
+        <v>12</v>
+      </c>
+      <c r="M44" t="s">
+        <v>0</v>
+      </c>
+      <c r="N44" s="4">
+        <v>7</v>
+      </c>
+      <c r="O44">
+        <v>4</v>
+      </c>
+      <c r="T44">
+        <v>9</v>
+      </c>
+      <c r="V44">
+        <v>8</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L45" s="4">
+        <v>9</v>
+      </c>
+      <c r="N45" s="4">
+        <v>7</v>
+      </c>
+      <c r="O45">
+        <v>4</v>
+      </c>
+      <c r="S45">
+        <v>6</v>
+      </c>
+      <c r="T45" t="s">
+        <v>15</v>
+      </c>
+      <c r="V45">
+        <v>8</v>
+      </c>
+      <c r="X45">
+        <v>12</v>
+      </c>
+      <c r="Z45">
+        <v>10</v>
+      </c>
+      <c r="AA45">
+        <v>3</v>
+      </c>
+      <c r="AB45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="I46">
+        <v>6</v>
+      </c>
+      <c r="K46" s="4">
+        <v>13</v>
+      </c>
+      <c r="L46" s="4">
+        <v>9</v>
+      </c>
+      <c r="N46" s="4">
+        <v>7</v>
+      </c>
+      <c r="O46">
+        <v>4</v>
+      </c>
+      <c r="S46">
+        <v>11</v>
+      </c>
+      <c r="V46" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z46">
+        <v>10</v>
+      </c>
+      <c r="AA46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="G47">
+        <v>11</v>
+      </c>
+      <c r="I47">
+        <v>6</v>
+      </c>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4">
+        <v>9</v>
+      </c>
+      <c r="N47" s="4">
+        <v>7</v>
+      </c>
+      <c r="O47">
+        <v>4</v>
+      </c>
+      <c r="V47">
+        <v>8</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA47">
+        <v>3</v>
+      </c>
+      <c r="AB47">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="I48">
+        <v>6</v>
+      </c>
+      <c r="J48">
+        <v>14</v>
+      </c>
+      <c r="K48" s="4">
+        <v>12</v>
+      </c>
+      <c r="L48" s="4">
+        <v>9</v>
+      </c>
+      <c r="N48" s="4">
+        <v>7</v>
+      </c>
+      <c r="O48">
+        <v>4</v>
+      </c>
+      <c r="S48" t="s">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>8</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <v>11</v>
+      </c>
+      <c r="I49">
+        <v>6</v>
+      </c>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N49" s="4">
+        <v>7</v>
+      </c>
+      <c r="O49">
+        <v>4</v>
+      </c>
+      <c r="S49">
+        <v>13</v>
+      </c>
+      <c r="V49">
+        <v>8</v>
+      </c>
+      <c r="Z49">
+        <v>14</v>
+      </c>
+      <c r="AA49">
+        <v>3</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>5</v>
+      </c>
+      <c r="G50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>6</v>
+      </c>
+      <c r="K50" s="4">
+        <v>12</v>
+      </c>
+      <c r="L50" s="4">
+        <v>9</v>
+      </c>
+      <c r="M50" t="s">
+        <v>46</v>
+      </c>
+      <c r="N50" s="4">
+        <v>7</v>
+      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
+      <c r="S50">
+        <v>13</v>
+      </c>
+      <c r="V50">
+        <v>8</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51">
+        <v>5</v>
+      </c>
+      <c r="J51" t="s">
+        <v>44</v>
+      </c>
+      <c r="K51" s="4">
+        <v>11</v>
+      </c>
+      <c r="L51" s="4">
+        <v>9</v>
+      </c>
+      <c r="N51" s="4">
+        <v>7</v>
+      </c>
+      <c r="O51">
+        <v>4</v>
+      </c>
+      <c r="S51">
+        <v>6</v>
+      </c>
+      <c r="T51">
+        <v>13</v>
+      </c>
+      <c r="V51">
+        <v>8</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB51">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>5</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>6</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L52" s="4">
+        <v>9</v>
+      </c>
+      <c r="N52" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="S52">
+        <v>12</v>
+      </c>
+      <c r="T52">
+        <v>13</v>
+      </c>
+      <c r="V52">
+        <v>8</v>
+      </c>
+      <c r="Z52">
+        <v>14</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>2</v>
+      </c>
+      <c r="C53">
+        <v>5</v>
+      </c>
+      <c r="G53">
+        <v>4</v>
+      </c>
+      <c r="H53">
+        <v>13</v>
+      </c>
+      <c r="I53" t="s">
+        <v>18</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="L53" s="4">
+        <v>9</v>
+      </c>
+      <c r="N53" s="4"/>
+      <c r="Q53" t="s">
+        <v>44</v>
+      </c>
+      <c r="R53">
+        <v>12</v>
+      </c>
+      <c r="S53">
+        <v>7</v>
+      </c>
+      <c r="T53">
+        <v>10</v>
+      </c>
+      <c r="V53">
+        <v>8</v>
+      </c>
+      <c r="Z53">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA77E507-ADE4-EC47-A9C7-E6FD7EAE7A4E}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed sub error in 85-86 games 46 and 47
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6991550-E198-7145-AC68-2BB5B0AFC2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2E106B-CE87-8741-BC86-DDC23844C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
   <sheets>
     <sheet name="1921-22" sheetId="19" r:id="rId1"/>
@@ -797,13 +797,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="HelveticaNeue"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -862,39 +868,42 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -916,9 +925,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -956,7 +965,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1062,7 +1071,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1204,7 +1213,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -28712,10 +28721,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D7BF1B0-6259-C248-A6FC-5199EE644BE5}">
   <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="V49" sqref="V49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -30492,8 +30501,8 @@
       <c r="U47" s="12">
         <v>6</v>
       </c>
-      <c r="V47" s="12" t="s">
-        <v>14</v>
+      <c r="V47" s="12">
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:22">
@@ -30527,8 +30536,8 @@
       <c r="U48" s="12">
         <v>6</v>
       </c>
-      <c r="V48" s="12">
-        <v>9</v>
+      <c r="V48" s="14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:22">
@@ -33427,8 +33436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82B88713-6708-F945-9EF9-BFF9276193B0}">
   <dimension ref="A1:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
edited 85-86 apps csv
</commit_message>
<xml_diff>
--- a/seasons/excel/scanning-seasons.xlsx
+++ b/seasons/excel/scanning-seasons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petebrown/Developer/complete-record/seasons/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B2E106B-CE87-8741-BC86-DDC23844C94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74201820-394E-354F-BB8B-7F7F1CFB5704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="4" xr2:uid="{47A77848-AA47-9549-8C92-1FFE5C0D5E8C}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2838" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2839" uniqueCount="246">
   <si>
     <t>11+</t>
   </si>
@@ -797,19 +797,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="HelveticaNeue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -868,43 +862,40 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -28724,7 +28715,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:A1048576"/>
-      <selection pane="bottomLeft" activeCell="V49" sqref="V49"/>
+      <selection pane="bottomLeft" sqref="A1:V56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -28733,2108 +28724,2664 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="O1" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="13" t="s">
         <v>237</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="R1" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="13" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:22">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="13">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12">
-        <v>3</v>
-      </c>
-      <c r="E2" s="12">
-        <v>10</v>
-      </c>
-      <c r="F2" s="12">
-        <v>4</v>
-      </c>
-      <c r="J2" s="12">
-        <v>6</v>
-      </c>
-      <c r="K2" s="12">
-        <v>7</v>
-      </c>
-      <c r="M2" s="12">
-        <v>12</v>
-      </c>
-      <c r="N2" s="12">
-        <v>2</v>
-      </c>
-      <c r="P2" s="12">
-        <v>5</v>
-      </c>
-      <c r="S2" s="12">
-        <v>8</v>
-      </c>
-      <c r="V2" s="12">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13">
+        <v>3</v>
+      </c>
+      <c r="E2" s="13">
+        <v>10</v>
+      </c>
+      <c r="F2" s="13">
+        <v>4</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13">
+        <v>6</v>
+      </c>
+      <c r="K2" s="13">
+        <v>7</v>
+      </c>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13">
+        <v>12</v>
+      </c>
+      <c r="N2" s="13">
+        <v>2</v>
+      </c>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13">
+        <v>8</v>
+      </c>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:22">
-      <c r="A3" s="12">
-        <v>1</v>
-      </c>
-      <c r="B3" s="12">
-        <v>11</v>
-      </c>
-      <c r="D3" s="12">
-        <v>3</v>
-      </c>
-      <c r="E3" s="12">
-        <v>10</v>
-      </c>
-      <c r="F3" s="12">
-        <v>4</v>
-      </c>
-      <c r="J3" s="12">
-        <v>6</v>
-      </c>
-      <c r="K3" s="12">
-        <v>7</v>
-      </c>
-      <c r="M3" s="12">
-        <v>12</v>
-      </c>
-      <c r="N3" s="12">
-        <v>2</v>
-      </c>
-      <c r="P3" s="12">
-        <v>5</v>
-      </c>
-      <c r="S3" s="12">
-        <v>8</v>
-      </c>
-      <c r="V3" s="12" t="s">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>11</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13">
+        <v>3</v>
+      </c>
+      <c r="E3" s="13">
+        <v>10</v>
+      </c>
+      <c r="F3" s="13">
+        <v>4</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13">
+        <v>6</v>
+      </c>
+      <c r="K3" s="13">
+        <v>7</v>
+      </c>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13">
+        <v>12</v>
+      </c>
+      <c r="N3" s="13">
+        <v>2</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13">
+        <v>8</v>
+      </c>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="12">
-        <v>1</v>
-      </c>
-      <c r="B4" s="12">
-        <v>11</v>
-      </c>
-      <c r="C4" s="12">
-        <v>12</v>
-      </c>
-      <c r="D4" s="12">
-        <v>3</v>
-      </c>
-      <c r="E4" s="12">
-        <v>10</v>
-      </c>
-      <c r="F4" s="12">
-        <v>4</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="A4" s="13">
+        <v>1</v>
+      </c>
+      <c r="B4" s="13">
+        <v>11</v>
+      </c>
+      <c r="C4" s="13">
+        <v>12</v>
+      </c>
+      <c r="D4" s="13">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>10</v>
+      </c>
+      <c r="F4" s="13">
+        <v>4</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="12">
-        <v>7</v>
-      </c>
-      <c r="N4" s="12">
-        <v>2</v>
-      </c>
-      <c r="P4" s="12">
-        <v>5</v>
-      </c>
-      <c r="S4" s="12">
-        <v>8</v>
-      </c>
-      <c r="V4" s="12">
+      <c r="K4" s="13">
+        <v>7</v>
+      </c>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13">
+        <v>2</v>
+      </c>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13">
+        <v>8</v>
+      </c>
+      <c r="T4" s="13"/>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="12">
-        <v>1</v>
-      </c>
-      <c r="B5" s="12">
-        <v>11</v>
-      </c>
-      <c r="C5" s="12">
-        <v>6</v>
-      </c>
-      <c r="D5" s="12">
-        <v>3</v>
-      </c>
-      <c r="F5" s="12">
-        <v>4</v>
-      </c>
-      <c r="K5" s="12" t="s">
+      <c r="A5" s="13">
+        <v>1</v>
+      </c>
+      <c r="B5" s="13">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13">
+        <v>6</v>
+      </c>
+      <c r="D5" s="13">
+        <v>3</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13">
+        <v>4</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="12">
-        <v>10</v>
-      </c>
-      <c r="N5" s="12">
-        <v>2</v>
-      </c>
-      <c r="P5" s="12">
-        <v>5</v>
-      </c>
-      <c r="R5" s="12">
-        <v>12</v>
-      </c>
-      <c r="S5" s="12">
-        <v>8</v>
-      </c>
-      <c r="V5" s="12">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13">
+        <v>10</v>
+      </c>
+      <c r="N5" s="13">
+        <v>2</v>
+      </c>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13">
+        <v>12</v>
+      </c>
+      <c r="S5" s="13">
+        <v>8</v>
+      </c>
+      <c r="T5" s="13"/>
+      <c r="U5" s="13"/>
+      <c r="V5" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="12">
-        <v>1</v>
-      </c>
-      <c r="B6" s="12">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12">
-        <v>10</v>
-      </c>
-      <c r="D6" s="12">
-        <v>3</v>
-      </c>
-      <c r="F6" s="12">
-        <v>4</v>
-      </c>
-      <c r="K6" s="12">
-        <v>12</v>
-      </c>
-      <c r="M6" s="12">
-        <v>7</v>
-      </c>
-      <c r="N6" s="12">
-        <v>6</v>
-      </c>
-      <c r="P6" s="12">
-        <v>5</v>
-      </c>
-      <c r="R6" s="12">
-        <v>2</v>
-      </c>
-      <c r="S6" s="12">
-        <v>8</v>
-      </c>
-      <c r="V6" s="12">
+      <c r="A6" s="13">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13">
+        <v>10</v>
+      </c>
+      <c r="D6" s="13">
+        <v>3</v>
+      </c>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13">
+        <v>4</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13">
+        <v>12</v>
+      </c>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13">
+        <v>7</v>
+      </c>
+      <c r="N6" s="13">
+        <v>6</v>
+      </c>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="13">
+        <v>2</v>
+      </c>
+      <c r="S6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" s="13"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="12">
-        <v>1</v>
-      </c>
-      <c r="B7" s="12">
-        <v>11</v>
-      </c>
-      <c r="C7" s="12">
-        <v>10</v>
-      </c>
-      <c r="D7" s="12">
-        <v>3</v>
-      </c>
-      <c r="F7" s="12">
-        <v>4</v>
-      </c>
-      <c r="J7" s="12">
-        <v>6</v>
-      </c>
-      <c r="M7" s="12">
-        <v>7</v>
-      </c>
-      <c r="N7" s="12">
-        <v>5</v>
-      </c>
-      <c r="R7" s="12">
-        <v>2</v>
-      </c>
-      <c r="S7" s="12">
-        <v>8</v>
-      </c>
-      <c r="V7" s="12">
+      <c r="A7" s="13">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>11</v>
+      </c>
+      <c r="C7" s="13">
+        <v>10</v>
+      </c>
+      <c r="D7" s="13">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13">
+        <v>4</v>
+      </c>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13">
+        <v>6</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13">
+        <v>7</v>
+      </c>
+      <c r="N7" s="13">
+        <v>5</v>
+      </c>
+      <c r="O7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13">
+        <v>2</v>
+      </c>
+      <c r="S7" s="13">
+        <v>8</v>
+      </c>
+      <c r="T7" s="13"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="12">
-        <v>1</v>
-      </c>
-      <c r="B8" s="12">
-        <v>11</v>
-      </c>
-      <c r="D8" s="12">
-        <v>3</v>
-      </c>
-      <c r="F8" s="12">
-        <v>4</v>
-      </c>
-      <c r="J8" s="12">
-        <v>6</v>
-      </c>
-      <c r="K8" s="12">
-        <v>10</v>
-      </c>
-      <c r="M8" s="12">
-        <v>7</v>
-      </c>
-      <c r="N8" s="12">
-        <v>5</v>
-      </c>
-      <c r="R8" s="12">
-        <v>2</v>
-      </c>
-      <c r="S8" s="12">
-        <v>8</v>
-      </c>
-      <c r="V8" s="12">
+      <c r="A8" s="13">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13">
+        <v>11</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13">
+        <v>3</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13">
+        <v>4</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13">
+        <v>6</v>
+      </c>
+      <c r="K8" s="13">
+        <v>10</v>
+      </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13">
+        <v>7</v>
+      </c>
+      <c r="N8" s="13">
+        <v>5</v>
+      </c>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13">
+        <v>2</v>
+      </c>
+      <c r="S8" s="13">
+        <v>8</v>
+      </c>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="12">
-        <v>1</v>
-      </c>
-      <c r="B9" s="12">
-        <v>11</v>
-      </c>
-      <c r="C9" s="12">
-        <v>12</v>
-      </c>
-      <c r="D9" s="12">
-        <v>3</v>
-      </c>
-      <c r="F9" s="12">
-        <v>4</v>
-      </c>
-      <c r="J9" s="12" t="s">
+      <c r="A9" s="13">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13">
+        <v>11</v>
+      </c>
+      <c r="C9" s="13">
+        <v>12</v>
+      </c>
+      <c r="D9" s="13">
+        <v>3</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13">
+        <v>4</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="12">
-        <v>10</v>
-      </c>
-      <c r="M9" s="12">
-        <v>7</v>
-      </c>
-      <c r="N9" s="12">
-        <v>5</v>
-      </c>
-      <c r="R9" s="12">
-        <v>2</v>
-      </c>
-      <c r="S9" s="12">
-        <v>8</v>
-      </c>
-      <c r="V9" s="12">
+      <c r="K9" s="13">
+        <v>10</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13">
+        <v>7</v>
+      </c>
+      <c r="N9" s="13">
+        <v>5</v>
+      </c>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13">
+        <v>2</v>
+      </c>
+      <c r="S9" s="13">
+        <v>8</v>
+      </c>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="12">
-        <v>1</v>
-      </c>
-      <c r="B10" s="12">
-        <v>11</v>
-      </c>
-      <c r="C10" s="12">
-        <v>5</v>
-      </c>
-      <c r="D10" s="12">
-        <v>3</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="A10" s="13">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13">
+        <v>11</v>
+      </c>
+      <c r="C10" s="13">
+        <v>5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>3</v>
+      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="12">
-        <v>6</v>
-      </c>
-      <c r="M10" s="12">
-        <v>10</v>
-      </c>
-      <c r="N10" s="12">
-        <v>2</v>
-      </c>
-      <c r="P10" s="12">
-        <v>12</v>
-      </c>
-      <c r="R10" s="12">
-        <v>7</v>
-      </c>
-      <c r="S10" s="12">
-        <v>8</v>
-      </c>
-      <c r="V10" s="12">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13">
+        <v>6</v>
+      </c>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13">
+        <v>10</v>
+      </c>
+      <c r="N10" s="13">
+        <v>2</v>
+      </c>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13">
+        <v>12</v>
+      </c>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13">
+        <v>7</v>
+      </c>
+      <c r="S10" s="13">
+        <v>8</v>
+      </c>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="12">
-        <v>1</v>
-      </c>
-      <c r="B11" s="12">
-        <v>11</v>
-      </c>
-      <c r="C11" s="12">
-        <v>5</v>
-      </c>
-      <c r="D11" s="12">
-        <v>3</v>
-      </c>
-      <c r="I11" s="12">
-        <v>4</v>
-      </c>
-      <c r="J11" s="12">
-        <v>6</v>
-      </c>
-      <c r="M11" s="12">
-        <v>10</v>
-      </c>
-      <c r="N11" s="12">
-        <v>2</v>
-      </c>
-      <c r="R11" s="12">
-        <v>7</v>
-      </c>
-      <c r="S11" s="12">
-        <v>8</v>
-      </c>
-      <c r="V11" s="12">
+      <c r="A11" s="13">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13">
+        <v>11</v>
+      </c>
+      <c r="C11" s="13">
+        <v>5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3</v>
+      </c>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13">
+        <v>4</v>
+      </c>
+      <c r="J11" s="13">
+        <v>6</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13">
+        <v>10</v>
+      </c>
+      <c r="N11" s="13">
+        <v>2</v>
+      </c>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13">
+        <v>7</v>
+      </c>
+      <c r="S11" s="13">
+        <v>8</v>
+      </c>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="12">
-        <v>1</v>
-      </c>
-      <c r="B12" s="12">
-        <v>11</v>
-      </c>
-      <c r="C12" s="12">
-        <v>5</v>
-      </c>
-      <c r="D12" s="12">
-        <v>3</v>
-      </c>
-      <c r="F12" s="12">
-        <v>6</v>
-      </c>
-      <c r="I12" s="12">
-        <v>4</v>
-      </c>
-      <c r="K12" s="12">
-        <v>12</v>
-      </c>
-      <c r="M12" s="12">
-        <v>10</v>
-      </c>
-      <c r="N12" s="12">
-        <v>2</v>
-      </c>
-      <c r="R12" s="12" t="s">
+      <c r="A12" s="13">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13">
+        <v>11</v>
+      </c>
+      <c r="C12" s="13">
+        <v>5</v>
+      </c>
+      <c r="D12" s="13">
+        <v>3</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13">
+        <v>6</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13">
+        <v>4</v>
+      </c>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13">
+        <v>12</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13">
+        <v>10</v>
+      </c>
+      <c r="N12" s="13">
+        <v>2</v>
+      </c>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="S12" s="12">
-        <v>8</v>
-      </c>
-      <c r="V12" s="12">
+      <c r="S12" s="13">
+        <v>8</v>
+      </c>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="12">
-        <v>1</v>
-      </c>
-      <c r="B13" s="12">
-        <v>11</v>
-      </c>
-      <c r="D13" s="12">
-        <v>3</v>
-      </c>
-      <c r="F13" s="12">
-        <v>6</v>
-      </c>
-      <c r="I13" s="12">
-        <v>4</v>
-      </c>
-      <c r="K13" s="12">
-        <v>5</v>
-      </c>
-      <c r="L13" s="12">
-        <v>7</v>
-      </c>
-      <c r="M13" s="12">
-        <v>10</v>
-      </c>
-      <c r="N13" s="12">
-        <v>2</v>
-      </c>
-      <c r="S13" s="12">
-        <v>8</v>
-      </c>
-      <c r="V13" s="12">
+      <c r="A13" s="13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13">
+        <v>11</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13">
+        <v>3</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13">
+        <v>6</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13">
+        <v>4</v>
+      </c>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13">
+        <v>5</v>
+      </c>
+      <c r="L13" s="13">
+        <v>7</v>
+      </c>
+      <c r="M13" s="13">
+        <v>10</v>
+      </c>
+      <c r="N13" s="13">
+        <v>2</v>
+      </c>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13">
+        <v>8</v>
+      </c>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:22">
       <c r="A14" s="13"/>
-      <c r="B14" s="12">
-        <v>11</v>
-      </c>
-      <c r="D14" s="12">
-        <v>3</v>
-      </c>
-      <c r="F14" s="12">
-        <v>6</v>
-      </c>
-      <c r="I14" s="12">
-        <v>4</v>
-      </c>
-      <c r="K14" s="12">
-        <v>5</v>
-      </c>
-      <c r="L14" s="12">
-        <v>7</v>
-      </c>
-      <c r="M14" s="12">
-        <v>10</v>
-      </c>
-      <c r="N14" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="12">
-        <v>1</v>
-      </c>
-      <c r="S14" s="12">
-        <v>8</v>
-      </c>
-      <c r="V14" s="12">
+      <c r="B14" s="13">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13">
+        <v>4</v>
+      </c>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13">
+        <v>5</v>
+      </c>
+      <c r="L14" s="13">
+        <v>7</v>
+      </c>
+      <c r="M14" s="13">
+        <v>10</v>
+      </c>
+      <c r="N14" s="13">
+        <v>2</v>
+      </c>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13">
+        <v>1</v>
+      </c>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13">
+        <v>8</v>
+      </c>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:22">
       <c r="A15" s="13"/>
-      <c r="B15" s="12">
-        <v>11</v>
-      </c>
-      <c r="D15" s="12">
-        <v>3</v>
-      </c>
-      <c r="F15" s="12">
-        <v>6</v>
-      </c>
-      <c r="I15" s="12">
-        <v>4</v>
-      </c>
-      <c r="K15" s="12">
-        <v>5</v>
-      </c>
-      <c r="L15" s="12">
-        <v>7</v>
-      </c>
-      <c r="M15" s="12">
-        <v>10</v>
-      </c>
-      <c r="N15" s="12">
-        <v>2</v>
-      </c>
-      <c r="P15" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="12">
-        <v>1</v>
-      </c>
-      <c r="V15" s="12">
+      <c r="B15" s="13">
+        <v>11</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13">
+        <v>3</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13">
+        <v>6</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13">
+        <v>4</v>
+      </c>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13">
+        <v>5</v>
+      </c>
+      <c r="L15" s="13">
+        <v>7</v>
+      </c>
+      <c r="M15" s="13">
+        <v>10</v>
+      </c>
+      <c r="N15" s="13">
+        <v>2</v>
+      </c>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="13">
+        <v>1</v>
+      </c>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:22">
       <c r="A16" s="13"/>
-      <c r="B16" s="12">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12">
-        <v>3</v>
-      </c>
-      <c r="F16" s="12">
-        <v>6</v>
-      </c>
-      <c r="I16" s="12">
-        <v>4</v>
-      </c>
-      <c r="K16" s="12">
-        <v>5</v>
-      </c>
-      <c r="L16" s="12">
-        <v>7</v>
-      </c>
-      <c r="M16" s="12">
-        <v>10</v>
-      </c>
-      <c r="N16" s="12">
-        <v>2</v>
-      </c>
-      <c r="P16" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q16" s="12">
-        <v>1</v>
-      </c>
-      <c r="V16" s="12">
+      <c r="B16" s="13">
+        <v>11</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13">
+        <v>3</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13">
+        <v>6</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13">
+        <v>4</v>
+      </c>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13">
+        <v>5</v>
+      </c>
+      <c r="L16" s="13">
+        <v>7</v>
+      </c>
+      <c r="M16" s="13">
+        <v>10</v>
+      </c>
+      <c r="N16" s="13">
+        <v>2</v>
+      </c>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="13">
+        <v>1</v>
+      </c>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:22">
       <c r="A17" s="13"/>
-      <c r="B17" s="12">
-        <v>11</v>
-      </c>
-      <c r="C17" s="12">
-        <v>12</v>
-      </c>
-      <c r="D17" s="12">
-        <v>3</v>
-      </c>
-      <c r="F17" s="12">
-        <v>6</v>
-      </c>
-      <c r="I17" s="12">
-        <v>4</v>
-      </c>
-      <c r="K17" s="12">
-        <v>5</v>
-      </c>
-      <c r="L17" s="12">
-        <v>7</v>
-      </c>
-      <c r="M17" s="12">
-        <v>10</v>
-      </c>
-      <c r="N17" s="12" t="s">
+      <c r="B17" s="13">
+        <v>11</v>
+      </c>
+      <c r="C17" s="13">
+        <v>12</v>
+      </c>
+      <c r="D17" s="13">
+        <v>3</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13">
+        <v>6</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13">
+        <v>4</v>
+      </c>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13">
+        <v>5</v>
+      </c>
+      <c r="L17" s="13">
+        <v>7</v>
+      </c>
+      <c r="M17" s="13">
+        <v>10</v>
+      </c>
+      <c r="N17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="P17" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q17" s="12">
-        <v>1</v>
-      </c>
-      <c r="V17" s="12">
+      <c r="O17" s="13"/>
+      <c r="P17" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>1</v>
+      </c>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:22">
       <c r="A18" s="13"/>
-      <c r="B18" s="12">
-        <v>11</v>
-      </c>
-      <c r="D18" s="12">
-        <v>3</v>
-      </c>
-      <c r="F18" s="12">
-        <v>6</v>
-      </c>
-      <c r="I18" s="12">
-        <v>4</v>
-      </c>
-      <c r="K18" s="12">
-        <v>5</v>
-      </c>
-      <c r="L18" s="12">
-        <v>7</v>
-      </c>
-      <c r="M18" s="12">
-        <v>10</v>
-      </c>
-      <c r="N18" s="12">
-        <v>2</v>
-      </c>
-      <c r="P18" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="12">
-        <v>1</v>
-      </c>
-      <c r="V18" s="12">
+      <c r="B18" s="13">
+        <v>11</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13">
+        <v>3</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13">
+        <v>4</v>
+      </c>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13">
+        <v>5</v>
+      </c>
+      <c r="L18" s="13">
+        <v>7</v>
+      </c>
+      <c r="M18" s="13">
+        <v>10</v>
+      </c>
+      <c r="N18" s="13">
+        <v>2</v>
+      </c>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>1</v>
+      </c>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:22">
       <c r="A19" s="13"/>
-      <c r="B19" s="12">
-        <v>11</v>
-      </c>
-      <c r="C19" s="12">
-        <v>12</v>
-      </c>
-      <c r="D19" s="12">
-        <v>3</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="12">
-        <v>4</v>
-      </c>
-      <c r="K19" s="12">
-        <v>5</v>
-      </c>
-      <c r="L19" s="12">
-        <v>7</v>
-      </c>
-      <c r="M19" s="12">
-        <v>10</v>
-      </c>
-      <c r="N19" s="12">
-        <v>2</v>
-      </c>
-      <c r="P19" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q19" s="12">
-        <v>1</v>
-      </c>
-      <c r="V19" s="12">
+      <c r="B19" s="13">
+        <v>11</v>
+      </c>
+      <c r="C19" s="13">
+        <v>12</v>
+      </c>
+      <c r="D19" s="13">
+        <v>3</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13">
+        <v>6</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13">
+        <v>4</v>
+      </c>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13">
+        <v>5</v>
+      </c>
+      <c r="L19" s="13">
+        <v>7</v>
+      </c>
+      <c r="M19" s="13">
+        <v>10</v>
+      </c>
+      <c r="N19" s="13">
+        <v>2</v>
+      </c>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q19" s="13">
+        <v>1</v>
+      </c>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:22">
       <c r="A20" s="13"/>
-      <c r="B20" s="12">
-        <v>11</v>
-      </c>
-      <c r="C20" s="12">
-        <v>12</v>
-      </c>
-      <c r="D20" s="12">
-        <v>3</v>
-      </c>
-      <c r="F20" s="12">
-        <v>6</v>
-      </c>
-      <c r="I20" s="12">
-        <v>4</v>
-      </c>
-      <c r="K20" s="12">
-        <v>5</v>
-      </c>
-      <c r="L20" s="12" t="s">
+      <c r="B20" s="13">
+        <v>11</v>
+      </c>
+      <c r="C20" s="13">
+        <v>12</v>
+      </c>
+      <c r="D20" s="13">
+        <v>3</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13">
+        <v>4</v>
+      </c>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13">
+        <v>5</v>
+      </c>
+      <c r="L20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="12">
-        <v>10</v>
-      </c>
-      <c r="N20" s="12">
-        <v>2</v>
-      </c>
-      <c r="P20" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q20" s="12">
-        <v>1</v>
-      </c>
-      <c r="V20" s="12">
+      <c r="M20" s="13">
+        <v>10</v>
+      </c>
+      <c r="N20" s="13">
+        <v>2</v>
+      </c>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q20" s="13">
+        <v>1</v>
+      </c>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:22">
       <c r="A21" s="13"/>
-      <c r="B21" s="12">
-        <v>11</v>
-      </c>
-      <c r="C21" s="12">
-        <v>5</v>
-      </c>
-      <c r="D21" s="12">
-        <v>3</v>
-      </c>
-      <c r="I21" s="12">
-        <v>4</v>
-      </c>
-      <c r="L21" s="12">
-        <v>7</v>
-      </c>
-      <c r="M21" s="12">
-        <v>10</v>
-      </c>
-      <c r="N21" s="12">
-        <v>2</v>
-      </c>
-      <c r="P21" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q21" s="12">
-        <v>1</v>
-      </c>
-      <c r="S21" s="12">
-        <v>6</v>
-      </c>
-      <c r="V21" s="12">
+      <c r="B21" s="13">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13">
+        <v>5</v>
+      </c>
+      <c r="D21" s="13">
+        <v>3</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13">
+        <v>6</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13">
+        <v>4</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13">
+        <v>7</v>
+      </c>
+      <c r="M21" s="13">
+        <v>10</v>
+      </c>
+      <c r="N21" s="13">
+        <v>2</v>
+      </c>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q21" s="13">
+        <v>1</v>
+      </c>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13">
+        <v>6</v>
+      </c>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:22">
       <c r="A22" s="13"/>
-      <c r="B22" s="12">
-        <v>11</v>
-      </c>
-      <c r="C22" s="12">
-        <v>5</v>
-      </c>
-      <c r="D22" s="12">
-        <v>3</v>
-      </c>
-      <c r="F22" s="12">
-        <v>6</v>
-      </c>
-      <c r="K22" s="12">
-        <v>4</v>
-      </c>
-      <c r="L22" s="12">
-        <v>7</v>
-      </c>
-      <c r="M22" s="12">
-        <v>10</v>
-      </c>
-      <c r="N22" s="12">
-        <v>2</v>
-      </c>
-      <c r="P22" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q22" s="12">
-        <v>1</v>
-      </c>
-      <c r="V22" s="12">
+      <c r="B22" s="13">
+        <v>11</v>
+      </c>
+      <c r="C22" s="13">
+        <v>5</v>
+      </c>
+      <c r="D22" s="13">
+        <v>3</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13">
+        <v>6</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13">
+        <v>4</v>
+      </c>
+      <c r="L22" s="13">
+        <v>7</v>
+      </c>
+      <c r="M22" s="13">
+        <v>10</v>
+      </c>
+      <c r="N22" s="13">
+        <v>2</v>
+      </c>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q22" s="13">
+        <v>1</v>
+      </c>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:22">
       <c r="A23" s="13"/>
-      <c r="B23" s="12">
-        <v>11</v>
-      </c>
-      <c r="C23" s="12">
-        <v>5</v>
-      </c>
-      <c r="D23" s="12">
-        <v>3</v>
-      </c>
-      <c r="F23" s="12">
-        <v>6</v>
-      </c>
-      <c r="K23" s="12">
-        <v>4</v>
-      </c>
-      <c r="L23" s="12">
-        <v>7</v>
-      </c>
-      <c r="M23" s="12">
-        <v>10</v>
-      </c>
-      <c r="N23" s="12">
-        <v>2</v>
-      </c>
-      <c r="P23" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q23" s="12">
-        <v>1</v>
-      </c>
-      <c r="V23" s="12">
+      <c r="B23" s="13">
+        <v>11</v>
+      </c>
+      <c r="C23" s="13">
+        <v>5</v>
+      </c>
+      <c r="D23" s="13">
+        <v>3</v>
+      </c>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13">
+        <v>6</v>
+      </c>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13">
+        <v>4</v>
+      </c>
+      <c r="L23" s="13">
+        <v>7</v>
+      </c>
+      <c r="M23" s="13">
+        <v>10</v>
+      </c>
+      <c r="N23" s="13">
+        <v>2</v>
+      </c>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q23" s="13">
+        <v>1</v>
+      </c>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:22">
       <c r="A24" s="13"/>
-      <c r="B24" s="12">
-        <v>11</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="12">
-        <v>3</v>
-      </c>
-      <c r="F24" s="12">
-        <v>6</v>
-      </c>
-      <c r="I24" s="12">
-        <v>12</v>
-      </c>
-      <c r="K24" s="12">
-        <v>4</v>
-      </c>
-      <c r="L24" s="12">
-        <v>7</v>
-      </c>
-      <c r="M24" s="12">
-        <v>10</v>
-      </c>
-      <c r="N24" s="12">
-        <v>2</v>
-      </c>
-      <c r="P24" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q24" s="12">
-        <v>1</v>
-      </c>
-      <c r="V24" s="12">
+      <c r="B24" s="13">
+        <v>11</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13">
+        <v>3</v>
+      </c>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13">
+        <v>12</v>
+      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13">
+        <v>4</v>
+      </c>
+      <c r="L24" s="13">
+        <v>7</v>
+      </c>
+      <c r="M24" s="13">
+        <v>10</v>
+      </c>
+      <c r="N24" s="13">
+        <v>2</v>
+      </c>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q24" s="13">
+        <v>1</v>
+      </c>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:22">
-      <c r="B25" s="12">
-        <v>11</v>
-      </c>
-      <c r="C25" s="12">
-        <v>9</v>
-      </c>
-      <c r="D25" s="12">
-        <v>3</v>
-      </c>
-      <c r="I25" s="12">
-        <v>5</v>
-      </c>
-      <c r="K25" s="12">
-        <v>4</v>
-      </c>
-      <c r="L25" s="12">
-        <v>7</v>
-      </c>
-      <c r="N25" s="12">
-        <v>2</v>
-      </c>
-      <c r="P25" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q25" s="12">
-        <v>1</v>
-      </c>
-      <c r="U25" s="12">
-        <v>6</v>
-      </c>
-      <c r="V25" s="12">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13">
+        <v>11</v>
+      </c>
+      <c r="C25" s="13">
+        <v>9</v>
+      </c>
+      <c r="D25" s="13">
+        <v>3</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13">
+        <v>5</v>
+      </c>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13">
+        <v>4</v>
+      </c>
+      <c r="L25" s="13">
+        <v>7</v>
+      </c>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13">
+        <v>2</v>
+      </c>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q25" s="13">
+        <v>1</v>
+      </c>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13">
+        <v>6</v>
+      </c>
+      <c r="V25" s="13">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:22">
-      <c r="B26" s="12">
-        <v>11</v>
-      </c>
-      <c r="C26" s="12">
-        <v>12</v>
-      </c>
-      <c r="D26" s="12">
-        <v>3</v>
-      </c>
-      <c r="I26" s="12">
-        <v>5</v>
-      </c>
-      <c r="K26" s="12">
-        <v>4</v>
-      </c>
-      <c r="L26" s="12">
-        <v>7</v>
-      </c>
-      <c r="N26" s="12" t="s">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13">
+        <v>11</v>
+      </c>
+      <c r="C26" s="13">
+        <v>12</v>
+      </c>
+      <c r="D26" s="13">
+        <v>3</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13">
+        <v>5</v>
+      </c>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13">
+        <v>4</v>
+      </c>
+      <c r="L26" s="13">
+        <v>7</v>
+      </c>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="P26" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q26" s="12">
-        <v>1</v>
-      </c>
-      <c r="S26" s="12">
-        <v>10</v>
-      </c>
-      <c r="U26" s="12">
-        <v>6</v>
-      </c>
-      <c r="V26" s="12">
+      <c r="O26" s="13"/>
+      <c r="P26" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="13">
+        <v>1</v>
+      </c>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13">
+        <v>10</v>
+      </c>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13">
+        <v>6</v>
+      </c>
+      <c r="V26" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:22">
-      <c r="B27" s="12">
-        <v>11</v>
-      </c>
-      <c r="D27" s="12">
-        <v>3</v>
-      </c>
-      <c r="I27" s="12">
-        <v>5</v>
-      </c>
-      <c r="K27" s="12">
-        <v>4</v>
-      </c>
-      <c r="L27" s="12">
-        <v>7</v>
-      </c>
-      <c r="N27" s="12">
-        <v>2</v>
-      </c>
-      <c r="P27" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q27" s="12">
-        <v>1</v>
-      </c>
-      <c r="S27" s="12">
-        <v>10</v>
-      </c>
-      <c r="U27" s="12">
-        <v>6</v>
-      </c>
-      <c r="V27" s="12">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13">
+        <v>11</v>
+      </c>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13">
+        <v>3</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13">
+        <v>5</v>
+      </c>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13">
+        <v>4</v>
+      </c>
+      <c r="L27" s="13">
+        <v>7</v>
+      </c>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13">
+        <v>2</v>
+      </c>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q27" s="13">
+        <v>1</v>
+      </c>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13">
+        <v>10</v>
+      </c>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13">
+        <v>6</v>
+      </c>
+      <c r="V27" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:22">
-      <c r="B28" s="12">
-        <v>11</v>
-      </c>
-      <c r="C28" s="12">
-        <v>12</v>
-      </c>
-      <c r="D28" s="12">
-        <v>3</v>
-      </c>
-      <c r="F28" s="12" t="s">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13">
+        <v>11</v>
+      </c>
+      <c r="C28" s="13">
+        <v>12</v>
+      </c>
+      <c r="D28" s="13">
+        <v>3</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13">
+        <v>5</v>
+      </c>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13">
+        <v>7</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13">
+        <v>2</v>
+      </c>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q28" s="13">
+        <v>1</v>
+      </c>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13">
+        <v>10</v>
+      </c>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13">
+        <v>6</v>
+      </c>
+      <c r="V28" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13">
+        <v>11</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13">
+        <v>3</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13">
+        <v>9</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13">
+        <v>5</v>
+      </c>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13">
+        <v>7</v>
+      </c>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13">
+        <v>2</v>
+      </c>
+      <c r="O29" s="13">
+        <v>10</v>
+      </c>
+      <c r="P29" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="13">
+        <v>1</v>
+      </c>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13">
+        <v>4</v>
+      </c>
+      <c r="T29" s="13"/>
+      <c r="U29" s="13">
+        <v>6</v>
+      </c>
+      <c r="V29" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="A30" s="13">
+        <v>1</v>
+      </c>
+      <c r="B30" s="13">
+        <v>11</v>
+      </c>
+      <c r="C30" s="13">
+        <v>12</v>
+      </c>
+      <c r="D30" s="13">
+        <v>3</v>
+      </c>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13">
+        <v>9</v>
+      </c>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13">
+        <v>5</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13">
+        <v>7</v>
+      </c>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13">
+        <v>2</v>
+      </c>
+      <c r="O30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="P30" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13">
+        <v>4</v>
+      </c>
+      <c r="T30" s="13"/>
+      <c r="U30" s="13">
+        <v>6</v>
+      </c>
+      <c r="V30" s="13"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="A31" s="13">
+        <v>1</v>
+      </c>
+      <c r="B31" s="13">
+        <v>11</v>
+      </c>
+      <c r="C31" s="13">
+        <v>5</v>
+      </c>
+      <c r="D31" s="13">
+        <v>3</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13">
+        <v>3</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13">
+        <v>7</v>
+      </c>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13">
+        <v>2</v>
+      </c>
+      <c r="O31" s="13">
+        <v>10</v>
+      </c>
+      <c r="P31" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13">
+        <v>4</v>
+      </c>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13">
+        <v>6</v>
+      </c>
+      <c r="V31" s="13"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="A32" s="13">
+        <v>1</v>
+      </c>
+      <c r="B32" s="13">
+        <v>11</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13">
+        <v>3</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13">
+        <v>12</v>
+      </c>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13">
+        <v>7</v>
+      </c>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13">
+        <v>2</v>
+      </c>
+      <c r="O32" s="13">
+        <v>10</v>
+      </c>
+      <c r="P32" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="13"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13">
+        <v>4</v>
+      </c>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13">
+        <v>6</v>
+      </c>
+      <c r="V32" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" s="13">
+        <v>1</v>
+      </c>
+      <c r="B33" s="13">
+        <v>11</v>
+      </c>
+      <c r="C33" s="13">
+        <v>5</v>
+      </c>
+      <c r="D33" s="13">
+        <v>12</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13">
+        <v>6</v>
+      </c>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13">
+        <v>4</v>
+      </c>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13">
+        <v>7</v>
+      </c>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13">
+        <v>2</v>
+      </c>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q33" s="13"/>
+      <c r="R33" s="13"/>
+      <c r="S33" s="13">
+        <v>10</v>
+      </c>
+      <c r="T33" s="13"/>
+      <c r="U33" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="V33" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22">
+      <c r="A34" s="13">
+        <v>1</v>
+      </c>
+      <c r="B34" s="13">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="13">
+        <v>3</v>
+      </c>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13">
+        <v>6</v>
+      </c>
+      <c r="G34" s="13">
+        <v>12</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13">
+        <v>4</v>
+      </c>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13">
+        <v>7</v>
+      </c>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13">
+        <v>2</v>
+      </c>
+      <c r="O34" s="13"/>
+      <c r="P34" s="13">
+        <v>8</v>
+      </c>
+      <c r="Q34" s="13"/>
+      <c r="R34" s="13"/>
+      <c r="S34" s="13">
+        <v>10</v>
+      </c>
+      <c r="T34" s="13"/>
+      <c r="U34" s="13"/>
+      <c r="V34" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" s="13">
+        <v>1</v>
+      </c>
+      <c r="B35" s="13">
+        <v>11</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13">
+        <v>3</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13">
+        <v>6</v>
+      </c>
+      <c r="G35" s="13">
+        <v>9</v>
+      </c>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13">
+        <v>4</v>
+      </c>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13">
+        <v>7</v>
+      </c>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13">
+        <v>2</v>
+      </c>
+      <c r="O35" s="13"/>
+      <c r="P35" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q35" s="13"/>
+      <c r="R35" s="13"/>
+      <c r="S35" s="13">
+        <v>8</v>
+      </c>
+      <c r="T35" s="13"/>
+      <c r="U35" s="13"/>
+      <c r="V35" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" s="13">
+        <v>1</v>
+      </c>
+      <c r="B36" s="13">
+        <v>11</v>
+      </c>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13">
+        <v>3</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13">
+        <v>6</v>
+      </c>
+      <c r="G36" s="13">
+        <v>9</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="12">
-        <v>5</v>
-      </c>
-      <c r="L28" s="12">
-        <v>7</v>
-      </c>
-      <c r="N28" s="12">
-        <v>2</v>
-      </c>
-      <c r="P28" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q28" s="12">
-        <v>1</v>
-      </c>
-      <c r="S28" s="12">
-        <v>10</v>
-      </c>
-      <c r="U28" s="12">
-        <v>6</v>
-      </c>
-      <c r="V28" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:22">
-      <c r="B29" s="12">
-        <v>11</v>
-      </c>
-      <c r="D29" s="12">
-        <v>3</v>
-      </c>
-      <c r="I29" s="12">
-        <v>5</v>
-      </c>
-      <c r="L29" s="12">
-        <v>7</v>
-      </c>
-      <c r="N29" s="12">
-        <v>2</v>
-      </c>
-      <c r="O29" s="12">
-        <v>10</v>
-      </c>
-      <c r="P29" s="12">
-        <v>8</v>
-      </c>
-      <c r="Q29" s="12">
-        <v>1</v>
-      </c>
-      <c r="S29" s="12">
-        <v>4</v>
-      </c>
-      <c r="U29" s="12">
-        <v>6</v>
-      </c>
-      <c r="V29" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="12">
-        <v>1</v>
-      </c>
-      <c r="B30" s="12">
-        <v>11</v>
-      </c>
-      <c r="C30" s="12">
-        <v>12</v>
-      </c>
-      <c r="D30" s="12">
-        <v>3</v>
-      </c>
-      <c r="F30" s="12">
-        <v>9</v>
-      </c>
-      <c r="I30" s="12">
-        <v>5</v>
-      </c>
-      <c r="L30" s="12">
-        <v>7</v>
-      </c>
-      <c r="N30" s="12">
-        <v>2</v>
-      </c>
-      <c r="O30" s="12" t="s">
+      <c r="J36" s="13"/>
+      <c r="K36" s="13">
+        <v>12</v>
+      </c>
+      <c r="L36" s="13">
+        <v>7</v>
+      </c>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13">
+        <v>2</v>
+      </c>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13">
+        <v>8</v>
+      </c>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" s="13">
+        <v>1</v>
+      </c>
+      <c r="B37" s="13">
+        <v>11</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13">
+        <v>6</v>
+      </c>
+      <c r="G37" s="13">
+        <v>9</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13">
+        <v>4</v>
+      </c>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+      <c r="L37" s="13">
+        <v>7</v>
+      </c>
+      <c r="M37" s="13">
+        <v>10</v>
+      </c>
+      <c r="N37" s="13">
+        <v>2</v>
+      </c>
+      <c r="O37" s="13"/>
+      <c r="P37" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q37" s="13"/>
+      <c r="R37" s="13"/>
+      <c r="S37" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13">
+        <v>3</v>
+      </c>
+      <c r="V37" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" s="13">
+        <v>1</v>
+      </c>
+      <c r="B38" s="13">
+        <v>11</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13">
+        <v>6</v>
+      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13">
+        <v>4</v>
+      </c>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13">
+        <v>12</v>
+      </c>
+      <c r="L38" s="13">
+        <v>7</v>
+      </c>
+      <c r="M38" s="13">
+        <v>10</v>
+      </c>
+      <c r="N38" s="13">
+        <v>2</v>
+      </c>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q38" s="13"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13">
+        <v>3</v>
+      </c>
+      <c r="V38" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39" s="13">
+        <v>1</v>
+      </c>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13">
+        <v>5</v>
+      </c>
+      <c r="D39" s="13">
+        <v>3</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13">
+        <v>6</v>
+      </c>
+      <c r="G39" s="13">
+        <v>9</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13">
+        <v>7</v>
+      </c>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13">
+        <v>10</v>
+      </c>
+      <c r="N39" s="13">
+        <v>2</v>
+      </c>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13">
+        <v>4</v>
+      </c>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13">
+        <v>8</v>
+      </c>
+      <c r="V39" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" s="13">
+        <v>1</v>
+      </c>
+      <c r="B40" s="13">
+        <v>11</v>
+      </c>
+      <c r="C40" s="13">
+        <v>5</v>
+      </c>
+      <c r="D40" s="13">
+        <v>3</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13">
+        <v>7</v>
+      </c>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+      <c r="L40" s="13"/>
+      <c r="M40" s="13">
+        <v>10</v>
+      </c>
+      <c r="N40" s="13">
+        <v>2</v>
+      </c>
+      <c r="O40" s="13"/>
+      <c r="P40" s="13"/>
+      <c r="Q40" s="13"/>
+      <c r="R40" s="13"/>
+      <c r="S40" s="13">
+        <v>4</v>
+      </c>
+      <c r="T40" s="13"/>
+      <c r="U40" s="13">
+        <v>8</v>
+      </c>
+      <c r="V40" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" s="13">
+        <v>1</v>
+      </c>
+      <c r="B41" s="13">
+        <v>11</v>
+      </c>
+      <c r="C41" s="13">
+        <v>9</v>
+      </c>
+      <c r="D41" s="13">
+        <v>3</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13">
+        <v>4</v>
+      </c>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13">
+        <v>7</v>
+      </c>
+      <c r="L41" s="13"/>
+      <c r="M41" s="13">
+        <v>10</v>
+      </c>
+      <c r="N41" s="13">
+        <v>2</v>
+      </c>
+      <c r="O41" s="13"/>
+      <c r="P41" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q41" s="13"/>
+      <c r="R41" s="13"/>
+      <c r="S41" s="13">
+        <v>8</v>
+      </c>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13">
+        <v>6</v>
+      </c>
+      <c r="V41" s="13"/>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" s="13">
+        <v>1</v>
+      </c>
+      <c r="B42" s="13">
+        <v>11</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="13">
+        <v>3</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13">
+        <v>4</v>
+      </c>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13">
+        <v>7</v>
+      </c>
+      <c r="L42" s="13"/>
+      <c r="M42" s="13">
+        <v>10</v>
+      </c>
+      <c r="N42" s="13">
+        <v>2</v>
+      </c>
+      <c r="O42" s="13"/>
+      <c r="P42" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q42" s="13"/>
+      <c r="R42" s="13"/>
+      <c r="S42" s="13">
+        <v>8</v>
+      </c>
+      <c r="T42" s="13"/>
+      <c r="U42" s="13">
+        <v>6</v>
+      </c>
+      <c r="V42" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" s="13">
+        <v>1</v>
+      </c>
+      <c r="B43" s="13">
+        <v>11</v>
+      </c>
+      <c r="C43" s="13">
+        <v>14</v>
+      </c>
+      <c r="D43" s="13">
+        <v>3</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13">
+        <v>4</v>
+      </c>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13">
+        <v>7</v>
+      </c>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13">
+        <v>10</v>
+      </c>
+      <c r="N43" s="13">
+        <v>2</v>
+      </c>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13">
+        <v>8</v>
+      </c>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="V43" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" s="13">
+        <v>1</v>
+      </c>
+      <c r="B44" s="13">
+        <v>11</v>
+      </c>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13">
+        <v>3</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13">
+        <v>4</v>
+      </c>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13">
+        <v>7</v>
+      </c>
+      <c r="L44" s="13">
+        <v>12</v>
+      </c>
+      <c r="M44" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="P30" s="12">
-        <v>8</v>
-      </c>
-      <c r="S30" s="12">
-        <v>4</v>
-      </c>
-      <c r="U30" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="12">
-        <v>1</v>
-      </c>
-      <c r="B31" s="12">
-        <v>11</v>
-      </c>
-      <c r="C31" s="12">
-        <v>5</v>
-      </c>
-      <c r="D31" s="12">
-        <v>3</v>
-      </c>
-      <c r="F31" s="12">
-        <v>9</v>
-      </c>
-      <c r="L31" s="12">
-        <v>7</v>
-      </c>
-      <c r="N31" s="12">
-        <v>2</v>
-      </c>
-      <c r="O31" s="12">
-        <v>10</v>
-      </c>
-      <c r="P31" s="12">
-        <v>8</v>
-      </c>
-      <c r="S31" s="12">
-        <v>4</v>
-      </c>
-      <c r="U31" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="12">
-        <v>1</v>
-      </c>
-      <c r="B32" s="12">
-        <v>11</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="12">
-        <v>3</v>
-      </c>
-      <c r="H32" s="12">
-        <v>12</v>
-      </c>
-      <c r="L32" s="12">
-        <v>7</v>
-      </c>
-      <c r="N32" s="12">
-        <v>2</v>
-      </c>
-      <c r="O32" s="12">
-        <v>10</v>
-      </c>
-      <c r="P32" s="12">
-        <v>8</v>
-      </c>
-      <c r="S32" s="12">
-        <v>4</v>
-      </c>
-      <c r="U32" s="12">
-        <v>6</v>
-      </c>
-      <c r="V32" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:22">
-      <c r="A33" s="12">
-        <v>1</v>
-      </c>
-      <c r="B33" s="12">
-        <v>11</v>
-      </c>
-      <c r="C33" s="12">
-        <v>5</v>
-      </c>
-      <c r="D33" s="12">
-        <v>12</v>
-      </c>
-      <c r="F33" s="12">
-        <v>3</v>
-      </c>
-      <c r="I33" s="12">
-        <v>4</v>
-      </c>
-      <c r="L33" s="12">
-        <v>7</v>
-      </c>
-      <c r="N33" s="12">
-        <v>2</v>
-      </c>
-      <c r="P33" s="12">
-        <v>8</v>
-      </c>
-      <c r="S33" s="12">
-        <v>10</v>
-      </c>
-      <c r="U33" s="12" t="s">
+      <c r="N44" s="13">
+        <v>2</v>
+      </c>
+      <c r="O44" s="13"/>
+      <c r="P44" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q44" s="13"/>
+      <c r="R44" s="13"/>
+      <c r="S44" s="13">
+        <v>8</v>
+      </c>
+      <c r="T44" s="13"/>
+      <c r="U44" s="13">
+        <v>6</v>
+      </c>
+      <c r="V44" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" s="13">
+        <v>1</v>
+      </c>
+      <c r="B45" s="13">
+        <v>11</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13">
+        <v>3</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13">
+        <v>4</v>
+      </c>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13">
+        <v>7</v>
+      </c>
+      <c r="L45" s="13">
+        <v>12</v>
+      </c>
+      <c r="M45" s="13">
+        <v>10</v>
+      </c>
+      <c r="N45" s="13">
+        <v>2</v>
+      </c>
+      <c r="O45" s="13"/>
+      <c r="P45" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q45" s="13"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13">
+        <v>6</v>
+      </c>
+      <c r="V45" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" s="13">
+        <v>1</v>
+      </c>
+      <c r="B46" s="13">
+        <v>11</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13">
+        <v>3</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13">
+        <v>4</v>
+      </c>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13">
+        <v>7</v>
+      </c>
+      <c r="L46" s="13"/>
+      <c r="M46" s="13">
+        <v>10</v>
+      </c>
+      <c r="N46" s="13">
+        <v>2</v>
+      </c>
+      <c r="O46" s="13"/>
+      <c r="P46" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q46" s="13"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13">
+        <v>8</v>
+      </c>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13">
+        <v>6</v>
+      </c>
+      <c r="V46" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" s="13">
+        <v>1</v>
+      </c>
+      <c r="B47" s="13">
+        <v>11</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13">
+        <v>3</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="J47" s="13"/>
+      <c r="K47" s="13">
+        <v>7</v>
+      </c>
+      <c r="L47" s="13">
+        <v>12</v>
+      </c>
+      <c r="M47" s="13">
+        <v>10</v>
+      </c>
+      <c r="N47" s="13">
+        <v>2</v>
+      </c>
+      <c r="O47" s="13"/>
+      <c r="P47" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q47" s="13"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13">
+        <v>8</v>
+      </c>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13">
+        <v>6</v>
+      </c>
+      <c r="V47" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" s="13">
+        <v>1</v>
+      </c>
+      <c r="B48" s="13">
+        <v>11</v>
+      </c>
+      <c r="C48" s="13">
+        <v>5</v>
+      </c>
+      <c r="D48" s="13">
+        <v>3</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13">
+        <v>12</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="13">
+        <v>8</v>
+      </c>
+      <c r="L48" s="13">
+        <v>7</v>
+      </c>
+      <c r="M48" s="13">
+        <v>10</v>
+      </c>
+      <c r="N48" s="13">
+        <v>2</v>
+      </c>
+      <c r="O48" s="13"/>
+      <c r="P48" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q48" s="13"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13">
+        <v>6</v>
+      </c>
+      <c r="V48" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" s="13">
+        <v>1</v>
+      </c>
+      <c r="B49" s="13">
+        <v>11</v>
+      </c>
+      <c r="C49" s="13">
+        <v>5</v>
+      </c>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="V33" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:22">
-      <c r="A34" s="12">
-        <v>1</v>
-      </c>
-      <c r="B34" s="12">
-        <v>11</v>
-      </c>
-      <c r="C34" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="12">
-        <v>3</v>
-      </c>
-      <c r="F34" s="12">
-        <v>6</v>
-      </c>
-      <c r="G34" s="12">
-        <v>12</v>
-      </c>
-      <c r="I34" s="12">
-        <v>4</v>
-      </c>
-      <c r="L34" s="12">
-        <v>7</v>
-      </c>
-      <c r="N34" s="12">
-        <v>2</v>
-      </c>
-      <c r="P34" s="12">
-        <v>8</v>
-      </c>
-      <c r="S34" s="12">
-        <v>10</v>
-      </c>
-      <c r="V34" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:22">
-      <c r="A35" s="12">
-        <v>1</v>
-      </c>
-      <c r="B35" s="12">
-        <v>11</v>
-      </c>
-      <c r="D35" s="12">
-        <v>3</v>
-      </c>
-      <c r="F35" s="12">
-        <v>6</v>
-      </c>
-      <c r="G35" s="12">
-        <v>9</v>
-      </c>
-      <c r="I35" s="12">
-        <v>4</v>
-      </c>
-      <c r="L35" s="12">
-        <v>7</v>
-      </c>
-      <c r="N35" s="12">
-        <v>2</v>
-      </c>
-      <c r="P35" s="12">
-        <v>5</v>
-      </c>
-      <c r="S35" s="12">
-        <v>8</v>
-      </c>
-      <c r="V35" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:22">
-      <c r="A36" s="12">
-        <v>1</v>
-      </c>
-      <c r="B36" s="12">
-        <v>11</v>
-      </c>
-      <c r="D36" s="12">
-        <v>3</v>
-      </c>
-      <c r="F36" s="12">
-        <v>6</v>
-      </c>
-      <c r="G36" s="12">
-        <v>9</v>
-      </c>
-      <c r="I36" s="12" t="s">
+      <c r="J49" s="13"/>
+      <c r="K49" s="13">
+        <v>7</v>
+      </c>
+      <c r="L49" s="13">
+        <v>12</v>
+      </c>
+      <c r="M49" s="13">
+        <v>10</v>
+      </c>
+      <c r="N49" s="13">
+        <v>2</v>
+      </c>
+      <c r="O49" s="13"/>
+      <c r="P49" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="13"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13">
+        <v>8</v>
+      </c>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13">
+        <v>3</v>
+      </c>
+      <c r="V49" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" s="13">
+        <v>1</v>
+      </c>
+      <c r="B50" s="13">
+        <v>11</v>
+      </c>
+      <c r="C50" s="13">
+        <v>5</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13">
+        <v>8</v>
+      </c>
+      <c r="G50" s="13">
+        <v>9</v>
+      </c>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13">
+        <v>12</v>
+      </c>
+      <c r="M50" s="13">
+        <v>10</v>
+      </c>
+      <c r="N50" s="13">
+        <v>2</v>
+      </c>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13">
+        <v>4</v>
+      </c>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="T50" s="13">
+        <v>6</v>
+      </c>
+      <c r="U50" s="13">
+        <v>3</v>
+      </c>
+      <c r="V50" s="13"/>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" s="13">
+        <v>1</v>
+      </c>
+      <c r="B51" s="13">
+        <v>11</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13">
+        <v>3</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13">
+        <v>8</v>
+      </c>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="13">
+        <v>7</v>
+      </c>
+      <c r="M51" s="13"/>
+      <c r="N51" s="13">
+        <v>2</v>
+      </c>
+      <c r="O51" s="13"/>
+      <c r="P51" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q51" s="13"/>
+      <c r="R51" s="13"/>
+      <c r="S51" s="13">
+        <v>10</v>
+      </c>
+      <c r="T51" s="13">
+        <v>4</v>
+      </c>
+      <c r="U51" s="13">
+        <v>6</v>
+      </c>
+      <c r="V51" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" s="13">
+        <v>1</v>
+      </c>
+      <c r="B52" s="13">
+        <v>11</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13">
+        <v>3</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13">
+        <v>4</v>
+      </c>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" s="13">
+        <v>7</v>
+      </c>
+      <c r="M52" s="13">
+        <v>12</v>
+      </c>
+      <c r="N52" s="13">
+        <v>2</v>
+      </c>
+      <c r="O52" s="13"/>
+      <c r="P52" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q52" s="13"/>
+      <c r="R52" s="13"/>
+      <c r="S52" s="13">
+        <v>10</v>
+      </c>
+      <c r="T52" s="13"/>
+      <c r="U52" s="13">
+        <v>6</v>
+      </c>
+      <c r="V52" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" s="13">
+        <v>1</v>
+      </c>
+      <c r="B53" s="13">
+        <v>11</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13">
+        <v>3</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13">
+        <v>8</v>
+      </c>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13">
+        <v>4</v>
+      </c>
+      <c r="J53" s="13"/>
+      <c r="K53" s="13"/>
+      <c r="L53" s="13">
+        <v>7</v>
+      </c>
+      <c r="M53" s="13"/>
+      <c r="N53" s="13">
+        <v>2</v>
+      </c>
+      <c r="O53" s="13"/>
+      <c r="P53" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q53" s="13"/>
+      <c r="R53" s="13"/>
+      <c r="S53" s="13">
+        <v>10</v>
+      </c>
+      <c r="T53" s="13"/>
+      <c r="U53" s="13">
+        <v>6</v>
+      </c>
+      <c r="V53" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" s="13">
+        <v>1</v>
+      </c>
+      <c r="B54" s="13">
+        <v>11</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13">
+        <v>3</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13">
+        <v>8</v>
+      </c>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13">
+        <v>4</v>
+      </c>
+      <c r="J54" s="13"/>
+      <c r="K54" s="13"/>
+      <c r="L54" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="M54" s="13">
+        <v>12</v>
+      </c>
+      <c r="N54" s="13">
+        <v>2</v>
+      </c>
+      <c r="O54" s="13"/>
+      <c r="P54" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q54" s="13"/>
+      <c r="R54" s="13"/>
+      <c r="S54" s="13">
+        <v>10</v>
+      </c>
+      <c r="T54" s="13"/>
+      <c r="U54" s="13">
+        <v>6</v>
+      </c>
+      <c r="V54" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55" s="13">
+        <v>1</v>
+      </c>
+      <c r="B55" s="13">
+        <v>11</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13">
+        <v>3</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13">
+        <v>8</v>
+      </c>
+      <c r="G55" s="13">
+        <v>12</v>
+      </c>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="13">
+        <v>7</v>
+      </c>
+      <c r="L55" s="13"/>
+      <c r="M55" s="13"/>
+      <c r="N55" s="13">
+        <v>2</v>
+      </c>
+      <c r="O55" s="13"/>
+      <c r="P55" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q55" s="13"/>
+      <c r="R55" s="13"/>
+      <c r="S55" s="13">
+        <v>10</v>
+      </c>
+      <c r="T55" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K36" s="12">
-        <v>12</v>
-      </c>
-      <c r="L36" s="12">
-        <v>7</v>
-      </c>
-      <c r="N36" s="12">
-        <v>2</v>
-      </c>
-      <c r="P36" s="12">
-        <v>5</v>
-      </c>
-      <c r="S36" s="12">
-        <v>8</v>
-      </c>
-      <c r="V36" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="12">
-        <v>1</v>
-      </c>
-      <c r="B37" s="12">
-        <v>11</v>
-      </c>
-      <c r="F37" s="12">
-        <v>6</v>
-      </c>
-      <c r="G37" s="12">
-        <v>9</v>
-      </c>
-      <c r="I37" s="12">
-        <v>4</v>
-      </c>
-      <c r="L37" s="12">
-        <v>7</v>
-      </c>
-      <c r="M37" s="12">
-        <v>10</v>
-      </c>
-      <c r="N37" s="12">
-        <v>2</v>
-      </c>
-      <c r="P37" s="12">
-        <v>5</v>
-      </c>
-      <c r="S37" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="U37" s="12">
-        <v>3</v>
-      </c>
-      <c r="V37" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22">
-      <c r="A38" s="12">
-        <v>1</v>
-      </c>
-      <c r="C38" s="12">
-        <v>5</v>
-      </c>
-      <c r="F38" s="12">
-        <v>6</v>
-      </c>
-      <c r="I38" s="12">
-        <v>4</v>
-      </c>
-      <c r="K38" s="12">
-        <v>12</v>
-      </c>
-      <c r="L38" s="12">
-        <v>7</v>
-      </c>
-      <c r="M38" s="12">
-        <v>10</v>
-      </c>
-      <c r="N38" s="12">
-        <v>2</v>
-      </c>
-      <c r="P38" s="12">
-        <v>5</v>
-      </c>
-      <c r="S38" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="U38" s="12">
-        <v>3</v>
-      </c>
-      <c r="V38" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:22">
-      <c r="A39" s="12">
-        <v>1</v>
-      </c>
-      <c r="B39" s="12">
-        <v>11</v>
-      </c>
-      <c r="C39" s="12">
-        <v>5</v>
-      </c>
-      <c r="D39" s="12">
-        <v>3</v>
-      </c>
-      <c r="F39" s="12">
-        <v>6</v>
-      </c>
-      <c r="G39" s="12">
-        <v>9</v>
-      </c>
-      <c r="K39" s="12">
-        <v>7</v>
-      </c>
-      <c r="M39" s="12">
-        <v>10</v>
-      </c>
-      <c r="N39" s="12">
-        <v>2</v>
-      </c>
-      <c r="S39" s="12">
-        <v>4</v>
-      </c>
-      <c r="U39" s="12">
-        <v>8</v>
-      </c>
-      <c r="V39" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:22">
-      <c r="A40" s="12">
-        <v>1</v>
-      </c>
-      <c r="B40" s="12">
-        <v>11</v>
-      </c>
-      <c r="C40" s="12">
-        <v>9</v>
-      </c>
-      <c r="D40" s="12">
-        <v>3</v>
-      </c>
-      <c r="F40" s="12">
-        <v>6</v>
-      </c>
-      <c r="I40" s="12">
-        <v>7</v>
-      </c>
-      <c r="M40" s="12">
-        <v>10</v>
-      </c>
-      <c r="N40" s="12">
-        <v>2</v>
-      </c>
-      <c r="S40" s="12">
-        <v>4</v>
-      </c>
-      <c r="U40" s="12">
-        <v>8</v>
-      </c>
-      <c r="V40" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
-      <c r="A41" s="12">
-        <v>1</v>
-      </c>
-      <c r="B41" s="12">
-        <v>11</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="12">
-        <v>3</v>
-      </c>
-      <c r="I41" s="12">
-        <v>4</v>
-      </c>
-      <c r="K41" s="12">
-        <v>7</v>
-      </c>
-      <c r="M41" s="12">
-        <v>10</v>
-      </c>
-      <c r="N41" s="12">
-        <v>2</v>
-      </c>
-      <c r="P41" s="12">
-        <v>5</v>
-      </c>
-      <c r="S41" s="12">
-        <v>8</v>
-      </c>
-      <c r="U41" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:22">
-      <c r="A42" s="12">
-        <v>1</v>
-      </c>
-      <c r="B42" s="12">
-        <v>11</v>
-      </c>
-      <c r="C42" s="12">
-        <v>14</v>
-      </c>
-      <c r="D42" s="12">
-        <v>3</v>
-      </c>
-      <c r="I42" s="12">
-        <v>4</v>
-      </c>
-      <c r="K42" s="12">
-        <v>7</v>
-      </c>
-      <c r="M42" s="12">
-        <v>10</v>
-      </c>
-      <c r="N42" s="12">
-        <v>2</v>
-      </c>
-      <c r="P42" s="12">
-        <v>5</v>
-      </c>
-      <c r="S42" s="12">
-        <v>8</v>
-      </c>
-      <c r="U42" s="12">
-        <v>6</v>
-      </c>
-      <c r="V42" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:22">
-      <c r="A43" s="12">
-        <v>1</v>
-      </c>
-      <c r="B43" s="12">
-        <v>11</v>
-      </c>
-      <c r="D43" s="12">
-        <v>3</v>
-      </c>
-      <c r="G43" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I43" s="12">
-        <v>4</v>
-      </c>
-      <c r="K43" s="12">
-        <v>7</v>
-      </c>
-      <c r="M43" s="12">
-        <v>10</v>
-      </c>
-      <c r="N43" s="12">
-        <v>2</v>
-      </c>
-      <c r="P43" s="12">
-        <v>5</v>
-      </c>
-      <c r="S43" s="12">
-        <v>8</v>
-      </c>
-      <c r="U43" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="V43" s="12">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:22">
-      <c r="A44" s="12">
-        <v>1</v>
-      </c>
-      <c r="B44" s="12">
-        <v>11</v>
-      </c>
-      <c r="D44" s="12">
-        <v>3</v>
-      </c>
-      <c r="I44" s="12">
-        <v>4</v>
-      </c>
-      <c r="K44" s="12">
-        <v>7</v>
-      </c>
-      <c r="L44" s="12">
-        <v>12</v>
-      </c>
-      <c r="M44" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="N44" s="12">
-        <v>2</v>
-      </c>
-      <c r="P44" s="12">
-        <v>5</v>
-      </c>
-      <c r="S44" s="12">
-        <v>8</v>
-      </c>
-      <c r="U44" s="12">
-        <v>6</v>
-      </c>
-      <c r="V44" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22">
-      <c r="A45" s="12">
-        <v>1</v>
-      </c>
-      <c r="B45" s="12">
-        <v>11</v>
-      </c>
-      <c r="D45" s="12">
-        <v>3</v>
-      </c>
-      <c r="I45" s="12">
-        <v>4</v>
-      </c>
-      <c r="K45" s="12">
-        <v>7</v>
-      </c>
-      <c r="L45" s="12">
-        <v>12</v>
-      </c>
-      <c r="M45" s="12">
-        <v>10</v>
-      </c>
-      <c r="N45" s="12">
-        <v>2</v>
-      </c>
-      <c r="P45" s="12">
-        <v>5</v>
-      </c>
-      <c r="S45" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="U45" s="12">
-        <v>6</v>
-      </c>
-      <c r="V45" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:22">
-      <c r="A46" s="12">
-        <v>1</v>
-      </c>
-      <c r="B46" s="12">
-        <v>11</v>
-      </c>
-      <c r="D46" s="12">
-        <v>3</v>
-      </c>
-      <c r="I46" s="12">
-        <v>4</v>
-      </c>
-      <c r="K46" s="12">
-        <v>7</v>
-      </c>
-      <c r="M46" s="12">
-        <v>10</v>
-      </c>
-      <c r="N46" s="12">
-        <v>2</v>
-      </c>
-      <c r="P46" s="12">
-        <v>5</v>
-      </c>
-      <c r="S46" s="12">
-        <v>8</v>
-      </c>
-      <c r="U46" s="12">
-        <v>6</v>
-      </c>
-      <c r="V46" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22">
-      <c r="A47" s="12">
-        <v>1</v>
-      </c>
-      <c r="B47" s="12">
-        <v>11</v>
-      </c>
-      <c r="C47" s="12">
-        <v>5</v>
-      </c>
-      <c r="D47" s="12">
-        <v>3</v>
-      </c>
-      <c r="I47" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="K47" s="12">
-        <v>7</v>
-      </c>
-      <c r="L47" s="12">
-        <v>12</v>
-      </c>
-      <c r="M47" s="12">
-        <v>10</v>
-      </c>
-      <c r="N47" s="12">
-        <v>2</v>
-      </c>
-      <c r="P47" s="12">
-        <v>5</v>
-      </c>
-      <c r="S47" s="12">
-        <v>8</v>
-      </c>
-      <c r="U47" s="12">
-        <v>6</v>
-      </c>
-      <c r="V47" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:22">
-      <c r="A48" s="12">
-        <v>1</v>
-      </c>
-      <c r="B48" s="12">
-        <v>11</v>
-      </c>
-      <c r="C48" s="12">
-        <v>5</v>
-      </c>
-      <c r="G48" s="12">
-        <v>12</v>
-      </c>
-      <c r="K48" s="12">
-        <v>8</v>
-      </c>
-      <c r="L48" s="12">
-        <v>7</v>
-      </c>
-      <c r="M48" s="12">
-        <v>10</v>
-      </c>
-      <c r="N48" s="12">
-        <v>2</v>
-      </c>
-      <c r="P48" s="12">
-        <v>4</v>
-      </c>
-      <c r="U48" s="12">
-        <v>6</v>
-      </c>
-      <c r="V48" s="14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="49" spans="1:22">
-      <c r="A49" s="12">
-        <v>1</v>
-      </c>
-      <c r="B49" s="12">
-        <v>11</v>
-      </c>
-      <c r="C49" s="12">
-        <v>5</v>
-      </c>
-      <c r="F49" s="12">
-        <v>8</v>
-      </c>
-      <c r="I49" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="K49" s="12">
-        <v>7</v>
-      </c>
-      <c r="L49" s="12">
-        <v>12</v>
-      </c>
-      <c r="M49" s="12">
-        <v>10</v>
-      </c>
-      <c r="N49" s="12">
-        <v>2</v>
-      </c>
-      <c r="P49" s="12">
-        <v>4</v>
-      </c>
-      <c r="S49" s="12">
-        <v>8</v>
-      </c>
-      <c r="U49" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="1:22">
-      <c r="A50" s="12">
-        <v>1</v>
-      </c>
-      <c r="B50" s="12">
-        <v>11</v>
-      </c>
-      <c r="D50" s="12">
-        <v>3</v>
-      </c>
-      <c r="F50" s="12">
-        <v>8</v>
-      </c>
-      <c r="G50" s="12">
-        <v>9</v>
-      </c>
-      <c r="L50" s="12">
-        <v>12</v>
-      </c>
-      <c r="M50" s="12">
-        <v>10</v>
-      </c>
-      <c r="N50" s="12">
-        <v>2</v>
-      </c>
-      <c r="P50" s="12">
-        <v>4</v>
-      </c>
-      <c r="S50" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="T50" s="12">
-        <v>6</v>
-      </c>
-      <c r="U50" s="12">
-        <v>3</v>
-      </c>
-      <c r="V50" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="51" spans="1:22">
-      <c r="A51" s="12">
-        <v>1</v>
-      </c>
-      <c r="B51" s="12">
-        <v>11</v>
-      </c>
-      <c r="D51" s="12">
-        <v>3</v>
-      </c>
-      <c r="F51" s="12">
-        <v>4</v>
-      </c>
-      <c r="L51" s="12">
-        <v>7</v>
-      </c>
-      <c r="N51" s="12">
-        <v>2</v>
-      </c>
-      <c r="P51" s="12">
-        <v>5</v>
-      </c>
-      <c r="S51" s="12">
-        <v>10</v>
-      </c>
-      <c r="T51" s="12">
-        <v>4</v>
-      </c>
-      <c r="U51" s="12">
-        <v>6</v>
-      </c>
-      <c r="V51" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="52" spans="1:22">
-      <c r="A52" s="12">
-        <v>1</v>
-      </c>
-      <c r="B52" s="12">
-        <v>11</v>
-      </c>
-      <c r="D52" s="12">
-        <v>3</v>
-      </c>
-      <c r="F52" s="12">
-        <v>8</v>
-      </c>
-      <c r="K52" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L52" s="12">
-        <v>7</v>
-      </c>
-      <c r="M52" s="12">
-        <v>12</v>
-      </c>
-      <c r="N52" s="12">
-        <v>2</v>
-      </c>
-      <c r="P52" s="12">
-        <v>5</v>
-      </c>
-      <c r="S52" s="12">
-        <v>10</v>
-      </c>
-      <c r="U52" s="12">
-        <v>6</v>
-      </c>
-      <c r="V52" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:22">
-      <c r="A53" s="12">
-        <v>1</v>
-      </c>
-      <c r="B53" s="12">
-        <v>11</v>
-      </c>
-      <c r="D53" s="12">
-        <v>3</v>
-      </c>
-      <c r="F53" s="12">
-        <v>8</v>
-      </c>
-      <c r="I53" s="12">
-        <v>4</v>
-      </c>
-      <c r="L53" s="12">
-        <v>7</v>
-      </c>
-      <c r="N53" s="12">
-        <v>2</v>
-      </c>
-      <c r="P53" s="12">
-        <v>5</v>
-      </c>
-      <c r="S53" s="12">
-        <v>10</v>
-      </c>
-      <c r="U53" s="12">
-        <v>6</v>
-      </c>
-      <c r="V53" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:22">
-      <c r="A54" s="12">
-        <v>1</v>
-      </c>
-      <c r="B54" s="12">
-        <v>11</v>
-      </c>
-      <c r="D54" s="12">
-        <v>3</v>
-      </c>
-      <c r="F54" s="12">
-        <v>8</v>
-      </c>
-      <c r="I54" s="12">
-        <v>4</v>
-      </c>
-      <c r="L54" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="M54" s="12">
-        <v>12</v>
-      </c>
-      <c r="N54" s="12">
-        <v>2</v>
-      </c>
-      <c r="P54" s="12">
-        <v>5</v>
-      </c>
-      <c r="S54" s="12">
-        <v>10</v>
-      </c>
-      <c r="U54" s="12">
-        <v>6</v>
-      </c>
-      <c r="V54" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:22">
-      <c r="A55" s="12">
-        <v>1</v>
-      </c>
-      <c r="B55" s="12">
-        <v>11</v>
-      </c>
-      <c r="D55" s="12">
-        <v>3</v>
-      </c>
-      <c r="F55" s="12">
-        <v>8</v>
-      </c>
-      <c r="G55" s="12">
-        <v>12</v>
-      </c>
-      <c r="K55" s="12">
-        <v>7</v>
-      </c>
-      <c r="N55" s="12">
-        <v>2</v>
-      </c>
-      <c r="P55" s="12">
-        <v>5</v>
-      </c>
-      <c r="S55" s="12">
-        <v>10</v>
-      </c>
-      <c r="T55" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="U55" s="12">
-        <v>6</v>
-      </c>
-      <c r="V55" s="12">
+      <c r="U55" s="13">
+        <v>6</v>
+      </c>
+      <c r="V55" s="13">
         <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:22">
-      <c r="A56" s="12">
-        <v>1</v>
-      </c>
-      <c r="B56" s="12">
-        <v>11</v>
-      </c>
-      <c r="D56" s="12">
-        <v>3</v>
-      </c>
-      <c r="F56" s="12">
-        <v>8</v>
-      </c>
-      <c r="G56" s="12">
-        <v>10</v>
-      </c>
-      <c r="I56" s="12">
-        <v>4</v>
-      </c>
-      <c r="L56" s="12">
-        <v>7</v>
-      </c>
-      <c r="N56" s="12">
-        <v>2</v>
-      </c>
-      <c r="P56" s="12">
-        <v>5</v>
-      </c>
-      <c r="U56" s="12">
-        <v>6</v>
-      </c>
-      <c r="V56" s="12">
+      <c r="A56" s="13">
+        <v>1</v>
+      </c>
+      <c r="B56" s="13">
+        <v>11</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13">
+        <v>3</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13">
+        <v>8</v>
+      </c>
+      <c r="G56" s="13">
+        <v>10</v>
+      </c>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13">
+        <v>4</v>
+      </c>
+      <c r="J56" s="13"/>
+      <c r="K56" s="13"/>
+      <c r="L56" s="13">
+        <v>7</v>
+      </c>
+      <c r="M56" s="13"/>
+      <c r="N56" s="13">
+        <v>2</v>
+      </c>
+      <c r="O56" s="13"/>
+      <c r="P56" s="13">
+        <v>5</v>
+      </c>
+      <c r="Q56" s="13"/>
+      <c r="R56" s="13"/>
+      <c r="S56" s="13"/>
+      <c r="T56" s="13"/>
+      <c r="U56" s="13">
+        <v>6</v>
+      </c>
+      <c r="V56" s="13">
         <v>9</v>
       </c>
     </row>

</xml_diff>